<commit_message>
fixed a snippet delivering title of first child item
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2SexyContent\Web\DesktopModules\ToSIC_SexyContent\src\sxc-develop\source-editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2sxc-ui\src\sxc-develop\source-editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11473"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475"/>
   </bookViews>
   <sheets>
     <sheet name="snippets" sheetId="1" r:id="rId1"/>
@@ -1651,9 +1651,6 @@
     <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Render() : "")</t>
   </si>
   <si>
-    <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Title : "")</t>
-  </si>
-  <si>
     <t>&lt;repeat repeat="${1:Employee} in Data:${2:Default}"&gt;...[${1}:Title]...&lt;/repeat&gt;</t>
   </si>
   <si>
@@ -1873,6 +1870,9 @@
   </si>
   <si>
     <t>read API docs: https://github.com/2sic/2sxc/wiki/Razor-Data</t>
+  </si>
+  <si>
+    <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].EntityTitle : "")</t>
   </si>
 </sst>
 </file>
@@ -2228,22 +2228,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="E256" sqref="E256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.46875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.64453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.52734375" customWidth="1"/>
-    <col min="5" max="5" width="54.41015625" customWidth="1"/>
-    <col min="6" max="6" width="40.52734375" customWidth="1"/>
-    <col min="7" max="7" width="44.234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2263,10 +2263,10 @@
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>477</v>
       </c>
@@ -2286,10 +2286,10 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>477</v>
       </c>
@@ -2309,10 +2309,10 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>477</v>
       </c>
@@ -2332,10 +2332,10 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>477</v>
       </c>
@@ -2355,10 +2355,10 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>477</v>
       </c>
@@ -2378,10 +2378,10 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>477</v>
       </c>
@@ -2401,10 +2401,10 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2412,19 +2412,19 @@
         <v>359</v>
       </c>
       <c r="C8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F8" t="s">
+        <v>594</v>
+      </c>
+      <c r="G8" t="s">
         <v>595</v>
       </c>
-      <c r="G8" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="43" hidden="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="9" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2432,19 +2432,19 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G9" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2452,19 +2452,19 @@
         <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G10" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2472,19 +2472,19 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G11" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2492,19 +2492,19 @@
         <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="F12" t="s">
         <v>555</v>
       </c>
-      <c r="F12" t="s">
-        <v>556</v>
-      </c>
       <c r="G12" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>458</v>
       </c>
@@ -2518,13 +2518,13 @@
         <v>307</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
@@ -2535,10 +2535,10 @@
         <v>456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="86" hidden="1" x14ac:dyDescent="0.5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2549,19 +2549,19 @@
         <v>461</v>
       </c>
       <c r="D15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="F15" t="s">
         <v>566</v>
       </c>
-      <c r="F15" t="s">
-        <v>567</v>
-      </c>
       <c r="G15" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2575,10 +2575,10 @@
         <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2592,10 +2592,10 @@
         <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2609,10 +2609,10 @@
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2626,10 +2626,10 @@
         <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2643,10 +2643,10 @@
         <v>39</v>
       </c>
       <c r="G20" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2660,10 +2660,10 @@
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2677,10 +2677,10 @@
         <v>43</v>
       </c>
       <c r="G22" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2694,10 +2694,10 @@
         <v>45</v>
       </c>
       <c r="G23" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2711,10 +2711,10 @@
         <v>47</v>
       </c>
       <c r="G24" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2728,10 +2728,10 @@
         <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2745,10 +2745,10 @@
         <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2762,10 +2762,10 @@
         <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2779,10 +2779,10 @@
         <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2796,10 +2796,10 @@
         <v>57</v>
       </c>
       <c r="G29" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2813,10 +2813,10 @@
         <v>59</v>
       </c>
       <c r="G30" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2830,10 +2830,10 @@
         <v>61</v>
       </c>
       <c r="G31" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2847,10 +2847,10 @@
         <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2864,10 +2864,10 @@
         <v>65</v>
       </c>
       <c r="G33" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2881,10 +2881,10 @@
         <v>67</v>
       </c>
       <c r="G34" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2898,10 +2898,10 @@
         <v>69</v>
       </c>
       <c r="G35" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2915,10 +2915,10 @@
         <v>71</v>
       </c>
       <c r="G36" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2932,10 +2932,10 @@
         <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2949,10 +2949,10 @@
         <v>75</v>
       </c>
       <c r="G38" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2966,10 +2966,10 @@
         <v>77</v>
       </c>
       <c r="G39" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2983,10 +2983,10 @@
         <v>79</v>
       </c>
       <c r="G40" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -3000,10 +3000,10 @@
         <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -3017,10 +3017,10 @@
         <v>83</v>
       </c>
       <c r="G42" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -3034,10 +3034,10 @@
         <v>85</v>
       </c>
       <c r="G43" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -3051,10 +3051,10 @@
         <v>87</v>
       </c>
       <c r="G44" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -3068,10 +3068,10 @@
         <v>89</v>
       </c>
       <c r="G45" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -3085,10 +3085,10 @@
         <v>91</v>
       </c>
       <c r="G46" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -3102,10 +3102,10 @@
         <v>93</v>
       </c>
       <c r="G47" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -3119,10 +3119,10 @@
         <v>95</v>
       </c>
       <c r="G48" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -3136,10 +3136,10 @@
         <v>97</v>
       </c>
       <c r="G49" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -3153,10 +3153,10 @@
         <v>99</v>
       </c>
       <c r="G50" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -3170,10 +3170,10 @@
         <v>101</v>
       </c>
       <c r="G51" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -3187,10 +3187,10 @@
         <v>103</v>
       </c>
       <c r="G52" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -3204,10 +3204,10 @@
         <v>104</v>
       </c>
       <c r="G53" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -3221,10 +3221,10 @@
         <v>105</v>
       </c>
       <c r="G54" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -3238,10 +3238,10 @@
         <v>107</v>
       </c>
       <c r="G55" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -3255,10 +3255,10 @@
         <v>109</v>
       </c>
       <c r="G56" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -3272,10 +3272,10 @@
         <v>111</v>
       </c>
       <c r="G57" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3289,10 +3289,10 @@
         <v>113</v>
       </c>
       <c r="G58" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3309,10 +3309,10 @@
         <v>440</v>
       </c>
       <c r="G59" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3326,10 +3326,10 @@
         <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3343,10 +3343,10 @@
         <v>118</v>
       </c>
       <c r="G61" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3360,10 +3360,10 @@
         <v>120</v>
       </c>
       <c r="G62" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3377,10 +3377,10 @@
         <v>122</v>
       </c>
       <c r="G63" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3394,10 +3394,10 @@
         <v>124</v>
       </c>
       <c r="G64" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3411,10 +3411,10 @@
         <v>126</v>
       </c>
       <c r="G65" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3428,10 +3428,10 @@
         <v>128</v>
       </c>
       <c r="G66" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3445,10 +3445,10 @@
         <v>130</v>
       </c>
       <c r="G67" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3462,10 +3462,10 @@
         <v>132</v>
       </c>
       <c r="G68" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3479,10 +3479,10 @@
         <v>134</v>
       </c>
       <c r="G69" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3496,10 +3496,10 @@
         <v>136</v>
       </c>
       <c r="G70" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3513,10 +3513,10 @@
         <v>138</v>
       </c>
       <c r="G71" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3530,10 +3530,10 @@
         <v>140</v>
       </c>
       <c r="G72" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3547,10 +3547,10 @@
         <v>142</v>
       </c>
       <c r="G73" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3564,10 +3564,10 @@
         <v>144</v>
       </c>
       <c r="G74" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3581,10 +3581,10 @@
         <v>146</v>
       </c>
       <c r="G75" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3598,10 +3598,10 @@
         <v>148</v>
       </c>
       <c r="G76" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3615,10 +3615,10 @@
         <v>149</v>
       </c>
       <c r="G77" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3632,10 +3632,10 @@
         <v>151</v>
       </c>
       <c r="G78" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3649,10 +3649,10 @@
         <v>153</v>
       </c>
       <c r="G79" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3666,10 +3666,10 @@
         <v>155</v>
       </c>
       <c r="G80" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3683,10 +3683,10 @@
         <v>157</v>
       </c>
       <c r="G81" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3700,10 +3700,10 @@
         <v>159</v>
       </c>
       <c r="G82" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3717,10 +3717,10 @@
         <v>160</v>
       </c>
       <c r="G83" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3734,10 +3734,10 @@
         <v>161</v>
       </c>
       <c r="G84" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3751,10 +3751,10 @@
         <v>163</v>
       </c>
       <c r="G85" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3768,10 +3768,10 @@
         <v>165</v>
       </c>
       <c r="G86" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3785,10 +3785,10 @@
         <v>167</v>
       </c>
       <c r="G87" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3802,10 +3802,10 @@
         <v>169</v>
       </c>
       <c r="G88" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3819,10 +3819,10 @@
         <v>171</v>
       </c>
       <c r="G89" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3836,10 +3836,10 @@
         <v>173</v>
       </c>
       <c r="G90" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3853,10 +3853,10 @@
         <v>175</v>
       </c>
       <c r="G91" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3870,10 +3870,10 @@
         <v>176</v>
       </c>
       <c r="G92" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3887,10 +3887,10 @@
         <v>178</v>
       </c>
       <c r="G93" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3904,10 +3904,10 @@
         <v>180</v>
       </c>
       <c r="G94" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3921,10 +3921,10 @@
         <v>182</v>
       </c>
       <c r="G95" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3938,10 +3938,10 @@
         <v>184</v>
       </c>
       <c r="G96" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3955,10 +3955,10 @@
         <v>186</v>
       </c>
       <c r="G97" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3972,10 +3972,10 @@
         <v>188</v>
       </c>
       <c r="G98" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3989,10 +3989,10 @@
         <v>189</v>
       </c>
       <c r="G99" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -4006,10 +4006,10 @@
         <v>191</v>
       </c>
       <c r="G100" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -4026,10 +4026,10 @@
         <v>309</v>
       </c>
       <c r="G101" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -4046,10 +4046,10 @@
         <v>310</v>
       </c>
       <c r="G102" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -4063,10 +4063,10 @@
         <v>197</v>
       </c>
       <c r="G103" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -4080,10 +4080,10 @@
         <v>199</v>
       </c>
       <c r="G104" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -4097,10 +4097,10 @@
         <v>201</v>
       </c>
       <c r="G105" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -4114,10 +4114,10 @@
         <v>203</v>
       </c>
       <c r="G106" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -4131,10 +4131,10 @@
         <v>204</v>
       </c>
       <c r="G107" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -4148,10 +4148,10 @@
         <v>206</v>
       </c>
       <c r="G108" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -4165,10 +4165,10 @@
         <v>208</v>
       </c>
       <c r="G109" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -4182,10 +4182,10 @@
         <v>210</v>
       </c>
       <c r="G110" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -4199,10 +4199,10 @@
         <v>212</v>
       </c>
       <c r="G111" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -4216,10 +4216,10 @@
         <v>214</v>
       </c>
       <c r="G112" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -4233,10 +4233,10 @@
         <v>216</v>
       </c>
       <c r="G113" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -4250,10 +4250,10 @@
         <v>218</v>
       </c>
       <c r="G114" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -4267,10 +4267,10 @@
         <v>220</v>
       </c>
       <c r="G115" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -4287,10 +4287,10 @@
         <v>311</v>
       </c>
       <c r="G116" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -4304,10 +4304,10 @@
         <v>223</v>
       </c>
       <c r="G117" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -4324,10 +4324,10 @@
         <v>312</v>
       </c>
       <c r="G118" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -4341,10 +4341,10 @@
         <v>227</v>
       </c>
       <c r="G119" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -4358,10 +4358,10 @@
         <v>229</v>
       </c>
       <c r="G120" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -4375,10 +4375,10 @@
         <v>231</v>
       </c>
       <c r="G121" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -4392,10 +4392,10 @@
         <v>233</v>
       </c>
       <c r="G122" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -4409,10 +4409,10 @@
         <v>235</v>
       </c>
       <c r="G123" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -4426,10 +4426,10 @@
         <v>237</v>
       </c>
       <c r="G124" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -4443,10 +4443,10 @@
         <v>239</v>
       </c>
       <c r="G125" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -4460,10 +4460,10 @@
         <v>241</v>
       </c>
       <c r="G126" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -4477,10 +4477,10 @@
         <v>243</v>
       </c>
       <c r="G127" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4497,10 +4497,10 @@
         <v>313</v>
       </c>
       <c r="G128" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4514,10 +4514,10 @@
         <v>247</v>
       </c>
       <c r="G129" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4531,10 +4531,10 @@
         <v>249</v>
       </c>
       <c r="G130" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4548,10 +4548,10 @@
         <v>251</v>
       </c>
       <c r="G131" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4565,10 +4565,10 @@
         <v>253</v>
       </c>
       <c r="G132" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4582,10 +4582,10 @@
         <v>255</v>
       </c>
       <c r="G133" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4599,10 +4599,10 @@
         <v>257</v>
       </c>
       <c r="G134" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4616,10 +4616,10 @@
         <v>259</v>
       </c>
       <c r="G135" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4633,10 +4633,10 @@
         <v>261</v>
       </c>
       <c r="G136" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4650,10 +4650,10 @@
         <v>263</v>
       </c>
       <c r="G137" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4667,10 +4667,10 @@
         <v>265</v>
       </c>
       <c r="G138" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4684,10 +4684,10 @@
         <v>267</v>
       </c>
       <c r="G139" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4701,10 +4701,10 @@
         <v>269</v>
       </c>
       <c r="G140" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4718,10 +4718,10 @@
         <v>271</v>
       </c>
       <c r="G141" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4735,10 +4735,10 @@
         <v>273</v>
       </c>
       <c r="G142" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4752,10 +4752,10 @@
         <v>275</v>
       </c>
       <c r="G143" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4769,10 +4769,10 @@
         <v>277</v>
       </c>
       <c r="G144" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4786,10 +4786,10 @@
         <v>279</v>
       </c>
       <c r="G145" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4803,10 +4803,10 @@
         <v>280</v>
       </c>
       <c r="G146" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4820,10 +4820,10 @@
         <v>282</v>
       </c>
       <c r="G147" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4837,10 +4837,10 @@
         <v>284</v>
       </c>
       <c r="G148" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4854,10 +4854,10 @@
         <v>285</v>
       </c>
       <c r="G149" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4871,10 +4871,10 @@
         <v>287</v>
       </c>
       <c r="G150" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4888,10 +4888,10 @@
         <v>289</v>
       </c>
       <c r="G151" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4905,10 +4905,10 @@
         <v>291</v>
       </c>
       <c r="G152" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4925,10 +4925,10 @@
         <v>314</v>
       </c>
       <c r="G153" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4942,10 +4942,10 @@
         <v>294</v>
       </c>
       <c r="G154" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4962,10 +4962,10 @@
         <v>315</v>
       </c>
       <c r="G155" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4979,10 +4979,10 @@
         <v>298</v>
       </c>
       <c r="G156" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4996,10 +4996,10 @@
         <v>300</v>
       </c>
       <c r="G157" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -5016,10 +5016,10 @@
         <v>316</v>
       </c>
       <c r="G158" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>441</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="86" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>441</v>
       </c>
@@ -5055,19 +5055,19 @@
         <v>474</v>
       </c>
       <c r="C161" t="s">
+        <v>585</v>
+      </c>
+      <c r="E161" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="F161" t="s">
         <v>587</v>
       </c>
-      <c r="F161" t="s">
-        <v>588</v>
-      </c>
       <c r="G161" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>441</v>
       </c>
@@ -5075,19 +5075,19 @@
         <v>474</v>
       </c>
       <c r="C162" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>289</v>
       </c>
       <c r="F162" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G162" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" ht="86" x14ac:dyDescent="0.5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>441</v>
       </c>
@@ -5095,16 +5095,16 @@
         <v>474</v>
       </c>
       <c r="C163" t="s">
+        <v>590</v>
+      </c>
+      <c r="E163" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="F163" t="s">
         <v>592</v>
       </c>
-      <c r="F163" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.5">
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>459</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>459</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>459</v>
       </c>
@@ -5185,41 +5185,41 @@
         <v>460</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B170" t="s">
+        <v>578</v>
+      </c>
+      <c r="C170" t="s">
         <v>579</v>
       </c>
-      <c r="C170" t="s">
-        <v>580</v>
-      </c>
       <c r="E170" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F170" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" ht="43" x14ac:dyDescent="0.5">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B171" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C171" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F171" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>355</v>
       </c>
@@ -5233,10 +5233,10 @@
         <v>319</v>
       </c>
       <c r="F172" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>355</v>
       </c>
@@ -5247,13 +5247,13 @@
         <v>361</v>
       </c>
       <c r="E173" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F173" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -5278,10 +5278,10 @@
         <v>456</v>
       </c>
       <c r="E175" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -5292,13 +5292,13 @@
         <v>321</v>
       </c>
       <c r="E176" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F176" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -5312,10 +5312,10 @@
         <v>323</v>
       </c>
       <c r="F177" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -5329,10 +5329,10 @@
         <v>325</v>
       </c>
       <c r="F178" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -5346,10 +5346,10 @@
         <v>327</v>
       </c>
       <c r="F179" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -5363,10 +5363,10 @@
         <v>329</v>
       </c>
       <c r="F180" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>356</v>
       </c>
@@ -5380,10 +5380,10 @@
         <v>331</v>
       </c>
       <c r="F181" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>356</v>
       </c>
@@ -5397,10 +5397,10 @@
         <v>333</v>
       </c>
       <c r="F182" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>356</v>
       </c>
@@ -5414,10 +5414,10 @@
         <v>335</v>
       </c>
       <c r="F183" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>356</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>356</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>478</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>478</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>478</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>478</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>478</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>478</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>357</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>357</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>357</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>357</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>357</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>423</v>
       </c>
@@ -6108,7 +6108,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>423</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>423</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>423</v>
       </c>
@@ -6159,7 +6159,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>423</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>424</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>424</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>424</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>424</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>424</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>464</v>
       </c>
@@ -6286,10 +6286,10 @@
         <v>468</v>
       </c>
       <c r="E235" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>484</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>484</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>466</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>466</v>
       </c>
@@ -6348,10 +6348,10 @@
         <v>468</v>
       </c>
       <c r="E239" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>479</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="129" x14ac:dyDescent="0.5">
+    <row r="241" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>479</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="242" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>479</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>479</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>479</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>479</v>
       </c>
@@ -6450,41 +6450,41 @@
         <v>502</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B246" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C246" t="s">
+        <v>574</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="F246" t="s">
         <v>575</v>
       </c>
-      <c r="E246" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="F246" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B247" t="s">
+        <v>570</v>
+      </c>
+      <c r="C247" t="s">
         <v>571</v>
       </c>
-      <c r="C247" t="s">
+      <c r="E247" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="E247" s="3" t="s">
+      <c r="F247" t="s">
         <v>573</v>
       </c>
-      <c r="F247" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
+    </row>
+    <row r="248" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>479</v>
       </c>
@@ -6495,13 +6495,13 @@
         <v>508</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F248" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="86" x14ac:dyDescent="0.5">
+    <row r="249" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>479</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="250" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>479</v>
       </c>
@@ -6529,13 +6529,13 @@
         <v>511</v>
       </c>
       <c r="E250" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F250" t="s">
         <v>569</v>
       </c>
-      <c r="F250" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>479</v>
       </c>
@@ -6546,13 +6546,13 @@
         <v>513</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F251" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>479</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>479</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>479</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>479</v>
       </c>
@@ -6614,13 +6614,13 @@
         <v>529</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>534</v>
+        <v>599</v>
       </c>
       <c r="F255" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
extended toolbars, edit template-settings works close https://github.com/2sic/2sxc/issues/998
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -1753,14 +1753,6 @@
     <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
-    <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
-    &lt;div class="sc-element"&gt;
-        @${1}.EntityTitle
-        @$Edit.Toolbar({1})
-    &lt;/div&gt;
-}</t>
-  </si>
-  <si>
     <t>simple loop to show all items in the default list</t>
   </si>
   <si>
@@ -1873,6 +1865,14 @@
   </si>
   <si>
     <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].EntityTitle : "")</t>
+  </si>
+  <si>
+    <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
+    &lt;div class="sc-element"&gt;
+        @${1}.EntityTitle
+        @Edit.Toolbar(${1})
+    &lt;/div&gt;
+}</t>
   </si>
 </sst>
 </file>
@@ -1936,20 +1936,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G256" totalsRowShown="0">
-  <autoFilter ref="A1:G256">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="@\InputType"/>
-        <filter val="@C#"/>
-        <filter val="@Html"/>
-        <filter val="@List"/>
-        <filter val="@User"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G256"/>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2228,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="E256" sqref="E256"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,10 +2250,10 @@
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>477</v>
       </c>
@@ -2286,10 +2273,10 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>477</v>
       </c>
@@ -2309,10 +2296,10 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>477</v>
       </c>
@@ -2332,10 +2319,10 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>477</v>
       </c>
@@ -2355,10 +2342,10 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>477</v>
       </c>
@@ -2378,10 +2365,10 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>477</v>
       </c>
@@ -2401,10 +2388,10 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2418,13 +2405,13 @@
         <v>547</v>
       </c>
       <c r="F8" t="s">
+        <v>593</v>
+      </c>
+      <c r="G8" t="s">
         <v>594</v>
       </c>
-      <c r="G8" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2441,10 +2428,10 @@
         <v>544</v>
       </c>
       <c r="G9" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2461,10 +2448,10 @@
         <v>551</v>
       </c>
       <c r="G10" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2481,10 +2468,10 @@
         <v>551</v>
       </c>
       <c r="G11" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2501,7 +2488,7 @@
         <v>555</v>
       </c>
       <c r="G12" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2538,7 +2525,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2549,19 +2536,19 @@
         <v>461</v>
       </c>
       <c r="D15" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="F15" t="s">
         <v>565</v>
       </c>
-      <c r="F15" t="s">
-        <v>566</v>
-      </c>
       <c r="G15" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2575,10 +2562,10 @@
         <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2592,10 +2579,10 @@
         <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2609,10 +2596,10 @@
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2626,10 +2613,10 @@
         <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2643,10 +2630,10 @@
         <v>39</v>
       </c>
       <c r="G20" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2660,10 +2647,10 @@
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2677,10 +2664,10 @@
         <v>43</v>
       </c>
       <c r="G22" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2694,10 +2681,10 @@
         <v>45</v>
       </c>
       <c r="G23" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2711,10 +2698,10 @@
         <v>47</v>
       </c>
       <c r="G24" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2728,10 +2715,10 @@
         <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2745,10 +2732,10 @@
         <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2762,10 +2749,10 @@
         <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2779,10 +2766,10 @@
         <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2796,10 +2783,10 @@
         <v>57</v>
       </c>
       <c r="G29" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2813,10 +2800,10 @@
         <v>59</v>
       </c>
       <c r="G30" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2830,10 +2817,10 @@
         <v>61</v>
       </c>
       <c r="G31" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2847,10 +2834,10 @@
         <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2864,10 +2851,10 @@
         <v>65</v>
       </c>
       <c r="G33" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2881,10 +2868,10 @@
         <v>67</v>
       </c>
       <c r="G34" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2898,10 +2885,10 @@
         <v>69</v>
       </c>
       <c r="G35" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2915,10 +2902,10 @@
         <v>71</v>
       </c>
       <c r="G36" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2932,10 +2919,10 @@
         <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2949,10 +2936,10 @@
         <v>75</v>
       </c>
       <c r="G38" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2966,10 +2953,10 @@
         <v>77</v>
       </c>
       <c r="G39" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2983,10 +2970,10 @@
         <v>79</v>
       </c>
       <c r="G40" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -3000,10 +2987,10 @@
         <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -3017,10 +3004,10 @@
         <v>83</v>
       </c>
       <c r="G42" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -3034,10 +3021,10 @@
         <v>85</v>
       </c>
       <c r="G43" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -3051,10 +3038,10 @@
         <v>87</v>
       </c>
       <c r="G44" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -3068,10 +3055,10 @@
         <v>89</v>
       </c>
       <c r="G45" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -3085,10 +3072,10 @@
         <v>91</v>
       </c>
       <c r="G46" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -3102,10 +3089,10 @@
         <v>93</v>
       </c>
       <c r="G47" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -3119,10 +3106,10 @@
         <v>95</v>
       </c>
       <c r="G48" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -3136,10 +3123,10 @@
         <v>97</v>
       </c>
       <c r="G49" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -3153,10 +3140,10 @@
         <v>99</v>
       </c>
       <c r="G50" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -3170,10 +3157,10 @@
         <v>101</v>
       </c>
       <c r="G51" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -3187,10 +3174,10 @@
         <v>103</v>
       </c>
       <c r="G52" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -3204,10 +3191,10 @@
         <v>104</v>
       </c>
       <c r="G53" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -3221,10 +3208,10 @@
         <v>105</v>
       </c>
       <c r="G54" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -3238,10 +3225,10 @@
         <v>107</v>
       </c>
       <c r="G55" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -3255,10 +3242,10 @@
         <v>109</v>
       </c>
       <c r="G56" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -3272,10 +3259,10 @@
         <v>111</v>
       </c>
       <c r="G57" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3289,10 +3276,10 @@
         <v>113</v>
       </c>
       <c r="G58" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3309,10 +3296,10 @@
         <v>440</v>
       </c>
       <c r="G59" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3326,10 +3313,10 @@
         <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3343,10 +3330,10 @@
         <v>118</v>
       </c>
       <c r="G61" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3360,10 +3347,10 @@
         <v>120</v>
       </c>
       <c r="G62" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3377,10 +3364,10 @@
         <v>122</v>
       </c>
       <c r="G63" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3394,10 +3381,10 @@
         <v>124</v>
       </c>
       <c r="G64" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3411,10 +3398,10 @@
         <v>126</v>
       </c>
       <c r="G65" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3428,10 +3415,10 @@
         <v>128</v>
       </c>
       <c r="G66" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3445,10 +3432,10 @@
         <v>130</v>
       </c>
       <c r="G67" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3462,10 +3449,10 @@
         <v>132</v>
       </c>
       <c r="G68" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3479,10 +3466,10 @@
         <v>134</v>
       </c>
       <c r="G69" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3496,10 +3483,10 @@
         <v>136</v>
       </c>
       <c r="G70" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3513,10 +3500,10 @@
         <v>138</v>
       </c>
       <c r="G71" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3530,10 +3517,10 @@
         <v>140</v>
       </c>
       <c r="G72" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3547,10 +3534,10 @@
         <v>142</v>
       </c>
       <c r="G73" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3564,10 +3551,10 @@
         <v>144</v>
       </c>
       <c r="G74" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3581,10 +3568,10 @@
         <v>146</v>
       </c>
       <c r="G75" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3598,10 +3585,10 @@
         <v>148</v>
       </c>
       <c r="G76" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3615,10 +3602,10 @@
         <v>149</v>
       </c>
       <c r="G77" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3632,10 +3619,10 @@
         <v>151</v>
       </c>
       <c r="G78" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3649,10 +3636,10 @@
         <v>153</v>
       </c>
       <c r="G79" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3666,10 +3653,10 @@
         <v>155</v>
       </c>
       <c r="G80" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3683,10 +3670,10 @@
         <v>157</v>
       </c>
       <c r="G81" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3700,10 +3687,10 @@
         <v>159</v>
       </c>
       <c r="G82" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3717,10 +3704,10 @@
         <v>160</v>
       </c>
       <c r="G83" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3734,10 +3721,10 @@
         <v>161</v>
       </c>
       <c r="G84" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3751,10 +3738,10 @@
         <v>163</v>
       </c>
       <c r="G85" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3768,10 +3755,10 @@
         <v>165</v>
       </c>
       <c r="G86" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3785,10 +3772,10 @@
         <v>167</v>
       </c>
       <c r="G87" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3802,10 +3789,10 @@
         <v>169</v>
       </c>
       <c r="G88" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3819,10 +3806,10 @@
         <v>171</v>
       </c>
       <c r="G89" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3836,10 +3823,10 @@
         <v>173</v>
       </c>
       <c r="G90" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3853,10 +3840,10 @@
         <v>175</v>
       </c>
       <c r="G91" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3870,10 +3857,10 @@
         <v>176</v>
       </c>
       <c r="G92" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3887,10 +3874,10 @@
         <v>178</v>
       </c>
       <c r="G93" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3904,10 +3891,10 @@
         <v>180</v>
       </c>
       <c r="G94" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3921,10 +3908,10 @@
         <v>182</v>
       </c>
       <c r="G95" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3938,10 +3925,10 @@
         <v>184</v>
       </c>
       <c r="G96" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3955,10 +3942,10 @@
         <v>186</v>
       </c>
       <c r="G97" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3972,10 +3959,10 @@
         <v>188</v>
       </c>
       <c r="G98" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3989,10 +3976,10 @@
         <v>189</v>
       </c>
       <c r="G99" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -4006,10 +3993,10 @@
         <v>191</v>
       </c>
       <c r="G100" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -4026,10 +4013,10 @@
         <v>309</v>
       </c>
       <c r="G101" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -4046,10 +4033,10 @@
         <v>310</v>
       </c>
       <c r="G102" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -4063,10 +4050,10 @@
         <v>197</v>
       </c>
       <c r="G103" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -4080,10 +4067,10 @@
         <v>199</v>
       </c>
       <c r="G104" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -4097,10 +4084,10 @@
         <v>201</v>
       </c>
       <c r="G105" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -4114,10 +4101,10 @@
         <v>203</v>
       </c>
       <c r="G106" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -4131,10 +4118,10 @@
         <v>204</v>
       </c>
       <c r="G107" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -4148,10 +4135,10 @@
         <v>206</v>
       </c>
       <c r="G108" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -4165,10 +4152,10 @@
         <v>208</v>
       </c>
       <c r="G109" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -4182,10 +4169,10 @@
         <v>210</v>
       </c>
       <c r="G110" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -4199,10 +4186,10 @@
         <v>212</v>
       </c>
       <c r="G111" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -4216,10 +4203,10 @@
         <v>214</v>
       </c>
       <c r="G112" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -4233,10 +4220,10 @@
         <v>216</v>
       </c>
       <c r="G113" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -4250,10 +4237,10 @@
         <v>218</v>
       </c>
       <c r="G114" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -4267,10 +4254,10 @@
         <v>220</v>
       </c>
       <c r="G115" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -4287,10 +4274,10 @@
         <v>311</v>
       </c>
       <c r="G116" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -4304,10 +4291,10 @@
         <v>223</v>
       </c>
       <c r="G117" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -4324,10 +4311,10 @@
         <v>312</v>
       </c>
       <c r="G118" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -4341,10 +4328,10 @@
         <v>227</v>
       </c>
       <c r="G119" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -4358,10 +4345,10 @@
         <v>229</v>
       </c>
       <c r="G120" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -4375,10 +4362,10 @@
         <v>231</v>
       </c>
       <c r="G121" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -4392,10 +4379,10 @@
         <v>233</v>
       </c>
       <c r="G122" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -4409,10 +4396,10 @@
         <v>235</v>
       </c>
       <c r="G123" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -4426,10 +4413,10 @@
         <v>237</v>
       </c>
       <c r="G124" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -4443,10 +4430,10 @@
         <v>239</v>
       </c>
       <c r="G125" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -4460,10 +4447,10 @@
         <v>241</v>
       </c>
       <c r="G126" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -4477,10 +4464,10 @@
         <v>243</v>
       </c>
       <c r="G127" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4497,10 +4484,10 @@
         <v>313</v>
       </c>
       <c r="G128" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4514,10 +4501,10 @@
         <v>247</v>
       </c>
       <c r="G129" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4531,10 +4518,10 @@
         <v>249</v>
       </c>
       <c r="G130" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4548,10 +4535,10 @@
         <v>251</v>
       </c>
       <c r="G131" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4565,10 +4552,10 @@
         <v>253</v>
       </c>
       <c r="G132" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4582,10 +4569,10 @@
         <v>255</v>
       </c>
       <c r="G133" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4599,10 +4586,10 @@
         <v>257</v>
       </c>
       <c r="G134" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4616,10 +4603,10 @@
         <v>259</v>
       </c>
       <c r="G135" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4633,10 +4620,10 @@
         <v>261</v>
       </c>
       <c r="G136" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4650,10 +4637,10 @@
         <v>263</v>
       </c>
       <c r="G137" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4667,10 +4654,10 @@
         <v>265</v>
       </c>
       <c r="G138" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4684,10 +4671,10 @@
         <v>267</v>
       </c>
       <c r="G139" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4701,10 +4688,10 @@
         <v>269</v>
       </c>
       <c r="G140" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4718,10 +4705,10 @@
         <v>271</v>
       </c>
       <c r="G141" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4735,10 +4722,10 @@
         <v>273</v>
       </c>
       <c r="G142" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4752,10 +4739,10 @@
         <v>275</v>
       </c>
       <c r="G143" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4769,10 +4756,10 @@
         <v>277</v>
       </c>
       <c r="G144" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4786,10 +4773,10 @@
         <v>279</v>
       </c>
       <c r="G145" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4803,10 +4790,10 @@
         <v>280</v>
       </c>
       <c r="G146" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4820,10 +4807,10 @@
         <v>282</v>
       </c>
       <c r="G147" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4837,10 +4824,10 @@
         <v>284</v>
       </c>
       <c r="G148" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4854,10 +4841,10 @@
         <v>285</v>
       </c>
       <c r="G149" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4871,10 +4858,10 @@
         <v>287</v>
       </c>
       <c r="G150" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4888,10 +4875,10 @@
         <v>289</v>
       </c>
       <c r="G151" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4905,10 +4892,10 @@
         <v>291</v>
       </c>
       <c r="G152" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4925,10 +4912,10 @@
         <v>314</v>
       </c>
       <c r="G153" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4942,10 +4929,10 @@
         <v>294</v>
       </c>
       <c r="G154" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4962,10 +4949,10 @@
         <v>315</v>
       </c>
       <c r="G155" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4979,10 +4966,10 @@
         <v>298</v>
       </c>
       <c r="G156" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4996,10 +4983,10 @@
         <v>300</v>
       </c>
       <c r="G157" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -5016,7 +5003,7 @@
         <v>316</v>
       </c>
       <c r="G158" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -5047,7 +5034,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>441</v>
       </c>
@@ -5055,19 +5042,19 @@
         <v>474</v>
       </c>
       <c r="C161" t="s">
+        <v>584</v>
+      </c>
+      <c r="E161" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="F161" t="s">
         <v>586</v>
       </c>
-      <c r="F161" t="s">
-        <v>587</v>
-      </c>
       <c r="G161" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>441</v>
       </c>
@@ -5075,16 +5062,16 @@
         <v>474</v>
       </c>
       <c r="C162" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>289</v>
       </c>
       <c r="F162" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G162" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -5095,13 +5082,13 @@
         <v>474</v>
       </c>
       <c r="C163" t="s">
+        <v>589</v>
+      </c>
+      <c r="E163" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="F163" t="s">
         <v>591</v>
-      </c>
-      <c r="F163" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5190,16 +5177,16 @@
         <v>459</v>
       </c>
       <c r="B170" t="s">
+        <v>577</v>
+      </c>
+      <c r="C170" t="s">
         <v>578</v>
       </c>
-      <c r="C170" t="s">
-        <v>579</v>
-      </c>
       <c r="E170" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F170" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -5207,19 +5194,19 @@
         <v>459</v>
       </c>
       <c r="B171" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C171" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F171" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>355</v>
       </c>
@@ -5236,7 +5223,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>355</v>
       </c>
@@ -5253,7 +5240,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -5267,7 +5254,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -5281,7 +5268,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -5298,7 +5285,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -5315,7 +5302,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -5332,7 +5319,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -5349,7 +5336,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -5366,7 +5353,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>356</v>
       </c>
@@ -5383,7 +5370,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>356</v>
       </c>
@@ -5400,7 +5387,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>356</v>
       </c>
@@ -5417,7 +5404,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>356</v>
       </c>
@@ -5431,7 +5418,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>356</v>
       </c>
@@ -5445,7 +5432,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>478</v>
       </c>
@@ -5462,7 +5449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>478</v>
       </c>
@@ -5479,7 +5466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>478</v>
       </c>
@@ -5496,7 +5483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>478</v>
       </c>
@@ -5513,7 +5500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>478</v>
       </c>
@@ -5530,7 +5517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>478</v>
       </c>
@@ -5547,7 +5534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -5564,7 +5551,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -5581,7 +5568,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5598,7 +5585,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5615,7 +5602,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5632,7 +5619,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5649,7 +5636,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5666,7 +5653,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5683,7 +5670,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5700,7 +5687,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5717,7 +5704,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5734,7 +5721,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5751,7 +5738,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5768,7 +5755,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5785,7 +5772,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5802,7 +5789,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5819,7 +5806,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5836,7 +5823,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5853,7 +5840,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5870,7 +5857,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5887,7 +5874,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5904,7 +5891,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5921,7 +5908,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5938,7 +5925,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5955,7 +5942,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5972,7 +5959,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>357</v>
       </c>
@@ -5989,7 +5976,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>357</v>
       </c>
@@ -6006,7 +5993,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>357</v>
       </c>
@@ -6023,7 +6010,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>357</v>
       </c>
@@ -6040,7 +6027,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>357</v>
       </c>
@@ -6057,7 +6044,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -6074,7 +6061,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -6091,7 +6078,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>423</v>
       </c>
@@ -6108,7 +6095,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>423</v>
       </c>
@@ -6125,7 +6112,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>423</v>
       </c>
@@ -6142,7 +6129,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>423</v>
       </c>
@@ -6159,7 +6146,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>423</v>
       </c>
@@ -6176,7 +6163,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>424</v>
       </c>
@@ -6193,7 +6180,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>424</v>
       </c>
@@ -6210,7 +6197,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>424</v>
       </c>
@@ -6227,7 +6214,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>424</v>
       </c>
@@ -6244,7 +6231,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>424</v>
       </c>
@@ -6261,7 +6248,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -6275,7 +6262,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>464</v>
       </c>
@@ -6289,7 +6276,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>484</v>
       </c>
@@ -6306,7 +6293,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>484</v>
       </c>
@@ -6455,16 +6442,16 @@
         <v>479</v>
       </c>
       <c r="B246" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C246" t="s">
+        <v>573</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F246" t="s">
         <v>574</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="F246" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -6472,16 +6459,16 @@
         <v>479</v>
       </c>
       <c r="B247" t="s">
+        <v>569</v>
+      </c>
+      <c r="C247" t="s">
         <v>570</v>
       </c>
-      <c r="C247" t="s">
+      <c r="E247" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="E247" s="3" t="s">
+      <c r="F247" t="s">
         <v>572</v>
-      </c>
-      <c r="F247" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -6529,10 +6516,10 @@
         <v>511</v>
       </c>
       <c r="E250" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="F250" t="s">
         <v>568</v>
-      </c>
-      <c r="F250" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -6614,7 +6601,7 @@
         <v>529</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F255" t="s">
         <v>530</v>

</xml_diff>

<commit_message>
Improved snippets for https://github.com/2sic/2sxc/issues/976
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="635">
   <si>
     <t>set</t>
   </si>
@@ -1917,6 +1917,75 @@
     <t>&lt;div class="sc-element"&gt;
     @Edit.Toolbar(${1:Content}, settings: new { classes = "${2:myCustomCssClass,anotherClass}" })
 &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>a script tag which enables scripts-combinations / packing etc. at default position &amp; priority</t>
+  </si>
+  <si>
+    <t>a script tag which enables scripts-combinations / packing etc. at lower priority in the header</t>
+  </si>
+  <si>
+    <t>&lt;script src="@App.Path/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="500:head"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>&lt;script src="@App.Path/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="bottom"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>a script tag which enables scripts-combinations / packing etc. at default priority at the bottom</t>
+  </si>
+  <si>
+    <t>&lt;script src="@App.Path/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="175:body"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>a script tag which enables scripts-combinations / packing etc. at custom priority at page-top (not header)</t>
+  </si>
+  <si>
+    <t>a css-tag which enables optimizations - with priority 100 (default) in def. position</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="body"/&gt;</t>
+  </si>
+  <si>
+    <t>a css-tag which enables optimizations - with priority default inside body</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="150:head"/&gt;</t>
+  </si>
+  <si>
+    <t>a css-tag which enables optimizations - with custom priority in head</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="bottom"/&gt;</t>
+  </si>
+  <si>
+    <t>a css-tag which enables optimizations - with def. priority at page bottom</t>
+  </si>
+  <si>
+    <t>read api-docs:https://github.com/2sic/2sxc/wiki/Template-Assets</t>
+  </si>
+  <si>
+    <t>script with optimization</t>
+  </si>
+  <si>
+    <t>script optimized into head</t>
+  </si>
+  <si>
+    <t>script optimized into bottom of page</t>
+  </si>
+  <si>
+    <t>script specifically in body</t>
+  </si>
+  <si>
+    <t>css, style-sheet with optimization</t>
+  </si>
+  <si>
+    <t>css, style-sheet loaded in body</t>
+  </si>
+  <si>
+    <t>css, style-sheet loaded in head</t>
+  </si>
+  <si>
+    <t>css, style-sheet loaded at bottom of page</t>
   </si>
 </sst>
 </file>
@@ -1979,8 +2048,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G260" totalsRowShown="0">
-  <autoFilter ref="A1:G260"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G266" totalsRowShown="0">
+  <autoFilter ref="A1:G266"/>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2257,10 +2326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G260"/>
+  <dimension ref="A1:G266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="C250" sqref="C250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6417,7 +6486,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>484</v>
       </c>
@@ -6434,7 +6503,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>466</v>
       </c>
@@ -6442,13 +6511,19 @@
         <v>462</v>
       </c>
       <c r="C242" t="s">
-        <v>463</v>
+        <v>627</v>
       </c>
       <c r="E242" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F242" t="s">
+        <v>612</v>
+      </c>
+      <c r="G242" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>466</v>
       </c>
@@ -6456,228 +6531,252 @@
         <v>462</v>
       </c>
       <c r="C243" t="s">
-        <v>468</v>
+        <v>628</v>
       </c>
       <c r="E243" t="s">
+        <v>614</v>
+      </c>
+      <c r="F243" t="s">
+        <v>613</v>
+      </c>
+      <c r="G243" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B244" t="s">
+        <v>462</v>
+      </c>
+      <c r="C244" t="s">
+        <v>629</v>
+      </c>
+      <c r="E244" t="s">
+        <v>615</v>
+      </c>
+      <c r="F244" t="s">
+        <v>616</v>
+      </c>
+      <c r="G244" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B245" t="s">
+        <v>462</v>
+      </c>
+      <c r="C245" t="s">
+        <v>630</v>
+      </c>
+      <c r="E245" t="s">
+        <v>617</v>
+      </c>
+      <c r="F245" t="s">
+        <v>618</v>
+      </c>
+      <c r="G245" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B246" t="s">
+        <v>462</v>
+      </c>
+      <c r="C246" t="s">
+        <v>631</v>
+      </c>
+      <c r="E246" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B244" t="s">
-        <v>480</v>
-      </c>
-      <c r="C244" t="s">
-        <v>488</v>
-      </c>
-      <c r="E244" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F244" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B245" t="s">
-        <v>480</v>
-      </c>
-      <c r="C245" t="s">
-        <v>489</v>
-      </c>
-      <c r="E245" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F245" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B246" t="s">
-        <v>480</v>
-      </c>
-      <c r="C246" t="s">
-        <v>491</v>
-      </c>
-      <c r="E246" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F246" t="s">
+        <v>619</v>
+      </c>
+      <c r="G246" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B247" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="C247" t="s">
-        <v>482</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>493</v>
+        <v>632</v>
+      </c>
+      <c r="E247" t="s">
+        <v>620</v>
       </c>
       <c r="F247" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+      <c r="G247" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B248" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="C248" t="s">
-        <v>483</v>
+        <v>633</v>
       </c>
       <c r="E248" t="s">
-        <v>494</v>
+        <v>622</v>
       </c>
       <c r="F248" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+      <c r="G248" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B249" t="s">
-        <v>499</v>
+        <v>462</v>
       </c>
       <c r="C249" t="s">
-        <v>500</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>501</v>
+        <v>634</v>
+      </c>
+      <c r="E249" t="s">
+        <v>624</v>
       </c>
       <c r="F249" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+      <c r="G249" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B250" t="s">
-        <v>575</v>
+        <v>480</v>
       </c>
       <c r="C250" t="s">
-        <v>572</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>574</v>
+        <v>488</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>497</v>
       </c>
       <c r="F250" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B251" t="s">
-        <v>568</v>
+        <v>480</v>
       </c>
       <c r="C251" t="s">
-        <v>569</v>
+        <v>489</v>
       </c>
       <c r="E251" s="3" t="s">
-        <v>570</v>
+        <v>498</v>
       </c>
       <c r="F251" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B252" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="C252" t="s">
-        <v>508</v>
-      </c>
-      <c r="E252" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="F252" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>491</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B253" t="s">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="C253" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F253" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+      <c r="F253" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B254" t="s">
-        <v>505</v>
+        <v>481</v>
       </c>
       <c r="C254" t="s">
-        <v>511</v>
-      </c>
-      <c r="E254" s="3" t="s">
-        <v>566</v>
+        <v>483</v>
+      </c>
+      <c r="E254" t="s">
+        <v>494</v>
       </c>
       <c r="F254" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B255" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C255" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>560</v>
+        <v>501</v>
       </c>
       <c r="F255" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B256" t="s">
-        <v>505</v>
+        <v>575</v>
       </c>
       <c r="C256" t="s">
-        <v>515</v>
+        <v>572</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>516</v>
+        <v>574</v>
       </c>
       <c r="F256" t="s">
-        <v>526</v>
+        <v>573</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
@@ -6685,66 +6784,168 @@
         <v>479</v>
       </c>
       <c r="B257" t="s">
-        <v>505</v>
+        <v>568</v>
       </c>
       <c r="C257" t="s">
-        <v>525</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>518</v>
+        <v>569</v>
+      </c>
+      <c r="E257" s="3" t="s">
+        <v>570</v>
       </c>
       <c r="F257" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B258" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C258" t="s">
-        <v>517</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>518</v>
+        <v>508</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>561</v>
       </c>
       <c r="F258" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B259" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C259" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="F259" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+      <c r="F259" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B260" t="s">
+        <v>505</v>
+      </c>
+      <c r="C260" t="s">
+        <v>511</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F260" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B261" t="s">
         <v>506</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C261" t="s">
+        <v>513</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F261" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B262" t="s">
+        <v>505</v>
+      </c>
+      <c r="C262" t="s">
+        <v>515</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="F262" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B263" t="s">
+        <v>505</v>
+      </c>
+      <c r="C263" t="s">
+        <v>525</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F263" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B264" t="s">
+        <v>505</v>
+      </c>
+      <c r="C264" t="s">
+        <v>517</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F264" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B265" t="s">
+        <v>505</v>
+      </c>
+      <c r="C265" t="s">
+        <v>529</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="F265" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B266" t="s">
+        <v>506</v>
+      </c>
+      <c r="C266" t="s">
         <v>531</v>
       </c>
-      <c r="E260" s="1" t="s">
+      <c r="E266" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F260" t="s">
+      <c r="F266" t="s">
         <v>532</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add snippet - close https://github.com/2sic/2sxc/issues/1091
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="638">
   <si>
     <t>set</t>
   </si>
@@ -1986,6 +1986,15 @@
   </si>
   <si>
     <t>css, style-sheet loaded at bottom of page</t>
+  </si>
+  <si>
+    <t>2sxc Scripts</t>
+  </si>
+  <si>
+    <t>standard 2sxc JS</t>
+  </si>
+  <si>
+    <t>&lt;script type="text/javascript" src="/desktopmodules/tosic_sexycontent/js/2sxc.api.min.js" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
@@ -2048,8 +2057,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G266" totalsRowShown="0">
-  <autoFilter ref="A1:G266"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G267" totalsRowShown="0">
+  <autoFilter ref="A1:G267"/>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2326,10 +2335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G266"/>
+  <dimension ref="A1:G267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="C250" sqref="C250"/>
+      <selection activeCell="E250" sqref="E250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6663,24 +6672,27 @@
         <v>626</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B250" t="s">
-        <v>480</v>
+        <v>635</v>
       </c>
       <c r="C250" t="s">
-        <v>488</v>
-      </c>
-      <c r="E250" s="3" t="s">
-        <v>497</v>
+        <v>636</v>
+      </c>
+      <c r="E250" t="s">
+        <v>637</v>
       </c>
       <c r="F250" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+      <c r="G250" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>479</v>
       </c>
@@ -6688,16 +6700,16 @@
         <v>480</v>
       </c>
       <c r="C251" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E251" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F251" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>479</v>
       </c>
@@ -6705,27 +6717,27 @@
         <v>480</v>
       </c>
       <c r="C252" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+      <c r="F252" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B253" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C253" t="s">
-        <v>482</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="F253" t="s">
-        <v>485</v>
+        <v>491</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -6736,13 +6748,13 @@
         <v>481</v>
       </c>
       <c r="C254" t="s">
-        <v>483</v>
-      </c>
-      <c r="E254" t="s">
-        <v>494</v>
+        <v>482</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>493</v>
       </c>
       <c r="F254" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -6750,16 +6762,16 @@
         <v>479</v>
       </c>
       <c r="B255" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="C255" t="s">
-        <v>500</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>501</v>
+        <v>483</v>
+      </c>
+      <c r="E255" t="s">
+        <v>494</v>
       </c>
       <c r="F255" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -6767,16 +6779,16 @@
         <v>479</v>
       </c>
       <c r="B256" t="s">
-        <v>575</v>
+        <v>499</v>
       </c>
       <c r="C256" t="s">
-        <v>572</v>
+        <v>500</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>574</v>
+        <v>501</v>
       </c>
       <c r="F256" t="s">
-        <v>573</v>
+        <v>502</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
@@ -6784,33 +6796,33 @@
         <v>479</v>
       </c>
       <c r="B257" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="C257" t="s">
-        <v>569</v>
-      </c>
-      <c r="E257" s="3" t="s">
-        <v>570</v>
+        <v>572</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>574</v>
       </c>
       <c r="F257" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B258" t="s">
-        <v>506</v>
+        <v>568</v>
       </c>
       <c r="C258" t="s">
-        <v>508</v>
-      </c>
-      <c r="E258" s="2" t="s">
-        <v>561</v>
+        <v>569</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>570</v>
       </c>
       <c r="F258" t="s">
-        <v>507</v>
+        <v>571</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -6821,47 +6833,47 @@
         <v>506</v>
       </c>
       <c r="C259" t="s">
-        <v>509</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F259" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="F259" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B260" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C260" t="s">
-        <v>511</v>
-      </c>
-      <c r="E260" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F260" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="F260" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B261" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C261" t="s">
-        <v>513</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>560</v>
+        <v>511</v>
+      </c>
+      <c r="E261" s="3" t="s">
+        <v>566</v>
       </c>
       <c r="F261" t="s">
-        <v>514</v>
+        <v>567</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
@@ -6869,16 +6881,16 @@
         <v>479</v>
       </c>
       <c r="B262" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C262" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>516</v>
+        <v>560</v>
       </c>
       <c r="F262" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
@@ -6889,13 +6901,13 @@
         <v>505</v>
       </c>
       <c r="C263" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F263" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
@@ -6906,13 +6918,13 @@
         <v>505</v>
       </c>
       <c r="C264" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="E264" s="1" t="s">
         <v>518</v>
       </c>
       <c r="F264" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
@@ -6923,13 +6935,13 @@
         <v>505</v>
       </c>
       <c r="C265" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>597</v>
+        <v>518</v>
       </c>
       <c r="F265" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
@@ -6937,15 +6949,32 @@
         <v>479</v>
       </c>
       <c r="B266" t="s">
+        <v>505</v>
+      </c>
+      <c r="C266" t="s">
+        <v>529</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="F266" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B267" t="s">
         <v>506</v>
       </c>
-      <c r="C266" t="s">
+      <c r="C267" t="s">
         <v>531</v>
       </c>
-      <c r="E266" s="1" t="s">
+      <c r="E267" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F266" t="s">
+      <c r="F267" t="s">
         <v>532</v>
       </c>
     </row>

</xml_diff>

<commit_message>
get i18n improved - part of https://github.com/2sic/2sxc/issues/1089
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="651">
   <si>
     <t>set</t>
   </si>
@@ -1789,9 +1789,6 @@
     <t>string-url-path</t>
   </si>
   <si>
-    <t>ASP.net Page</t>
-  </si>
-  <si>
     <t>Set page title</t>
   </si>
   <si>
@@ -1988,13 +1985,57 @@
     <t>css, style-sheet loaded at bottom of page</t>
   </si>
   <si>
-    <t>2sxc Scripts</t>
-  </si>
-  <si>
     <t>standard 2sxc JS</t>
   </si>
   <si>
     <t>&lt;script type="text/javascript" src="/desktopmodules/tosic_sexycontent/js/2sxc.api.min.js" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>@ToSic.SexyContent.ContentBlocks.Render.All(${1:Content}, field: "${2:ContentBlocks}")</t>
+  </si>
+  <si>
+    <t>Render Very-Rich-Text</t>
+  </si>
+  <si>
+    <t>Render Virtual Pane on this item</t>
+  </si>
+  <si>
+    <t>Create an area, into which the editor can add apps/content-blocks</t>
+  </si>
+  <si>
+    <t>Render a wysiwyg-field containing content-block placeholders</t>
+  </si>
+  <si>
+    <t>read api-docs:https://github.com/2sic/2sxc/wiki/Razor-Content-Blocks
+tutorial blog:http://2sxc.org/en/blog/post/designing-articles-with-inner-content-blocks-new-in-8-4-like-modules-inside-modules</t>
+  </si>
+  <si>
+    <t>read api-docs:https://github.com/2sic/2sxc/wiki/Razor-Content-Blocks
+tutorial very-rich-text:http://2sxc.org/en/blog/post/tutorial-create-very-rich-text-inner-content-2-with-2sxc</t>
+  </si>
+  <si>
+    <t>@ToSic.SexyContent.ContentBlocks.Render.All(${1:Content}, field: "${2:BodyContentBlocks}", merge: ${3:Content.Body})</t>
+  </si>
+  <si>
+    <t>InnerContent</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>2sxcScripts</t>
+  </si>
+  <si>
+    <t>2sxc Angular1 JS</t>
+  </si>
+  <si>
+    <t>read api-docs:https://github.com/2sic/2sxc/wiki/AngularJs-1-Overview</t>
+  </si>
+  <si>
+    <t>angular1 - remember to also include the 2sxc</t>
+  </si>
+  <si>
+    <t>&lt;script type="text/javascript" src="/desktopmodules/tosic_sexycontent/js/angularjs/angular.min.js" data-enableoptimizations="101"&gt;&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2071,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2039,6 +2080,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2057,8 +2099,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G267" totalsRowShown="0">
-  <autoFilter ref="A1:G267"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G270" totalsRowShown="0">
+  <autoFilter ref="A1:G270"/>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2335,10 +2377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G267"/>
+  <dimension ref="A1:G270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="E250" sqref="E250"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="G253" sqref="G253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2372,7 +2414,7 @@
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2394,8 +2436,8 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
-        <v>595</v>
+      <c r="G2" s="4" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2417,8 +2459,8 @@
       <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="G3" t="s">
-        <v>595</v>
+      <c r="G3" s="4" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2440,8 +2482,8 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
-        <v>595</v>
+      <c r="G4" s="4" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2463,8 +2505,8 @@
       <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
-        <v>595</v>
+      <c r="G5" s="4" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2486,8 +2528,8 @@
       <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
-        <v>595</v>
+      <c r="G6" s="4" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2509,8 +2551,8 @@
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
-        <v>595</v>
+      <c r="G7" s="4" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2527,10 +2569,10 @@
         <v>547</v>
       </c>
       <c r="F8" t="s">
+        <v>591</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="G8" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2541,7 +2583,7 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>548</v>
@@ -2549,8 +2591,8 @@
       <c r="F9" t="s">
         <v>544</v>
       </c>
-      <c r="G9" t="s">
-        <v>593</v>
+      <c r="G9" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2561,16 +2603,16 @@
         <v>359</v>
       </c>
       <c r="C10" t="s">
+        <v>599</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>601</v>
-      </c>
       <c r="F10" t="s">
-        <v>605</v>
-      </c>
-      <c r="G10" t="s">
-        <v>593</v>
+        <v>604</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2581,16 +2623,16 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
+        <v>601</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>603</v>
-      </c>
       <c r="F11" t="s">
-        <v>606</v>
-      </c>
-      <c r="G11" t="s">
-        <v>593</v>
+        <v>605</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2601,16 +2643,16 @@
         <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F12" t="s">
-        <v>607</v>
-      </c>
-      <c r="G12" t="s">
-        <v>593</v>
+        <v>606</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2621,16 +2663,16 @@
         <v>359</v>
       </c>
       <c r="C13" t="s">
+        <v>608</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="F13" t="s">
         <v>609</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="F13" t="s">
-        <v>610</v>
-      </c>
-      <c r="G13" t="s">
-        <v>593</v>
+      <c r="G13" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2649,8 +2691,8 @@
       <c r="F14" t="s">
         <v>551</v>
       </c>
-      <c r="G14" t="s">
-        <v>593</v>
+      <c r="G14" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2669,8 +2711,8 @@
       <c r="F15" t="s">
         <v>551</v>
       </c>
-      <c r="G15" t="s">
-        <v>593</v>
+      <c r="G15" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2689,8 +2731,8 @@
       <c r="F16" t="s">
         <v>555</v>
       </c>
-      <c r="G16" t="s">
-        <v>593</v>
+      <c r="G16" s="4" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2712,6 +2754,7 @@
       <c r="F17" t="s">
         <v>308</v>
       </c>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2726,6 +2769,7 @@
       <c r="E18" s="2" t="s">
         <v>550</v>
       </c>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -2741,13 +2785,13 @@
         <v>565</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F19" t="s">
         <v>564</v>
       </c>
-      <c r="G19" t="s">
-        <v>596</v>
+      <c r="G19" s="4" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2763,8 +2807,8 @@
       <c r="E20" t="s">
         <v>31</v>
       </c>
-      <c r="G20" t="s">
-        <v>594</v>
+      <c r="G20" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2780,8 +2824,8 @@
       <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="G21" t="s">
-        <v>594</v>
+      <c r="G21" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2797,8 +2841,8 @@
       <c r="E22" t="s">
         <v>35</v>
       </c>
-      <c r="G22" t="s">
-        <v>594</v>
+      <c r="G22" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,8 +2858,8 @@
       <c r="E23" t="s">
         <v>37</v>
       </c>
-      <c r="G23" t="s">
-        <v>594</v>
+      <c r="G23" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2831,8 +2875,8 @@
       <c r="E24" t="s">
         <v>39</v>
       </c>
-      <c r="G24" t="s">
-        <v>594</v>
+      <c r="G24" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2848,8 +2892,8 @@
       <c r="E25" t="s">
         <v>41</v>
       </c>
-      <c r="G25" t="s">
-        <v>594</v>
+      <c r="G25" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2865,8 +2909,8 @@
       <c r="E26" t="s">
         <v>43</v>
       </c>
-      <c r="G26" t="s">
-        <v>594</v>
+      <c r="G26" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2882,8 +2926,8 @@
       <c r="E27" t="s">
         <v>45</v>
       </c>
-      <c r="G27" t="s">
-        <v>594</v>
+      <c r="G27" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2899,8 +2943,8 @@
       <c r="E28" t="s">
         <v>47</v>
       </c>
-      <c r="G28" t="s">
-        <v>594</v>
+      <c r="G28" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,8 +2960,8 @@
       <c r="E29" t="s">
         <v>49</v>
       </c>
-      <c r="G29" t="s">
-        <v>594</v>
+      <c r="G29" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2933,8 +2977,8 @@
       <c r="E30" t="s">
         <v>51</v>
       </c>
-      <c r="G30" t="s">
-        <v>594</v>
+      <c r="G30" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2950,8 +2994,8 @@
       <c r="E31" t="s">
         <v>53</v>
       </c>
-      <c r="G31" t="s">
-        <v>594</v>
+      <c r="G31" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2967,8 +3011,8 @@
       <c r="E32" t="s">
         <v>55</v>
       </c>
-      <c r="G32" t="s">
-        <v>594</v>
+      <c r="G32" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2984,8 +3028,8 @@
       <c r="E33" t="s">
         <v>57</v>
       </c>
-      <c r="G33" t="s">
-        <v>594</v>
+      <c r="G33" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3001,8 +3045,8 @@
       <c r="E34" t="s">
         <v>59</v>
       </c>
-      <c r="G34" t="s">
-        <v>594</v>
+      <c r="G34" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3018,8 +3062,8 @@
       <c r="E35" t="s">
         <v>61</v>
       </c>
-      <c r="G35" t="s">
-        <v>594</v>
+      <c r="G35" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,8 +3079,8 @@
       <c r="E36" t="s">
         <v>63</v>
       </c>
-      <c r="G36" t="s">
-        <v>594</v>
+      <c r="G36" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3052,8 +3096,8 @@
       <c r="E37" t="s">
         <v>65</v>
       </c>
-      <c r="G37" t="s">
-        <v>594</v>
+      <c r="G37" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3069,8 +3113,8 @@
       <c r="E38" t="s">
         <v>67</v>
       </c>
-      <c r="G38" t="s">
-        <v>594</v>
+      <c r="G38" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3086,8 +3130,8 @@
       <c r="E39" t="s">
         <v>69</v>
       </c>
-      <c r="G39" t="s">
-        <v>594</v>
+      <c r="G39" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3103,8 +3147,8 @@
       <c r="E40" t="s">
         <v>71</v>
       </c>
-      <c r="G40" t="s">
-        <v>594</v>
+      <c r="G40" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3120,8 +3164,8 @@
       <c r="E41" t="s">
         <v>73</v>
       </c>
-      <c r="G41" t="s">
-        <v>594</v>
+      <c r="G41" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3137,8 +3181,8 @@
       <c r="E42" t="s">
         <v>75</v>
       </c>
-      <c r="G42" t="s">
-        <v>594</v>
+      <c r="G42" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3154,8 +3198,8 @@
       <c r="E43" t="s">
         <v>77</v>
       </c>
-      <c r="G43" t="s">
-        <v>594</v>
+      <c r="G43" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3171,8 +3215,8 @@
       <c r="E44" t="s">
         <v>79</v>
       </c>
-      <c r="G44" t="s">
-        <v>594</v>
+      <c r="G44" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3188,8 +3232,8 @@
       <c r="E45" t="s">
         <v>81</v>
       </c>
-      <c r="G45" t="s">
-        <v>594</v>
+      <c r="G45" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3205,8 +3249,8 @@
       <c r="E46" t="s">
         <v>83</v>
       </c>
-      <c r="G46" t="s">
-        <v>594</v>
+      <c r="G46" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3222,8 +3266,8 @@
       <c r="E47" t="s">
         <v>85</v>
       </c>
-      <c r="G47" t="s">
-        <v>594</v>
+      <c r="G47" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3239,8 +3283,8 @@
       <c r="E48" t="s">
         <v>87</v>
       </c>
-      <c r="G48" t="s">
-        <v>594</v>
+      <c r="G48" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3256,8 +3300,8 @@
       <c r="E49" t="s">
         <v>89</v>
       </c>
-      <c r="G49" t="s">
-        <v>594</v>
+      <c r="G49" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3273,8 +3317,8 @@
       <c r="E50" t="s">
         <v>91</v>
       </c>
-      <c r="G50" t="s">
-        <v>594</v>
+      <c r="G50" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3290,8 +3334,8 @@
       <c r="E51" t="s">
         <v>93</v>
       </c>
-      <c r="G51" t="s">
-        <v>594</v>
+      <c r="G51" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3307,8 +3351,8 @@
       <c r="E52" t="s">
         <v>95</v>
       </c>
-      <c r="G52" t="s">
-        <v>594</v>
+      <c r="G52" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3324,8 +3368,8 @@
       <c r="E53" t="s">
         <v>97</v>
       </c>
-      <c r="G53" t="s">
-        <v>594</v>
+      <c r="G53" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3341,8 +3385,8 @@
       <c r="E54" t="s">
         <v>99</v>
       </c>
-      <c r="G54" t="s">
-        <v>594</v>
+      <c r="G54" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3358,8 +3402,8 @@
       <c r="E55" t="s">
         <v>101</v>
       </c>
-      <c r="G55" t="s">
-        <v>594</v>
+      <c r="G55" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3375,8 +3419,8 @@
       <c r="E56" t="s">
         <v>103</v>
       </c>
-      <c r="G56" t="s">
-        <v>594</v>
+      <c r="G56" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3392,8 +3436,8 @@
       <c r="E57" t="s">
         <v>104</v>
       </c>
-      <c r="G57" t="s">
-        <v>594</v>
+      <c r="G57" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3409,8 +3453,8 @@
       <c r="E58" t="s">
         <v>105</v>
       </c>
-      <c r="G58" t="s">
-        <v>594</v>
+      <c r="G58" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3426,8 +3470,8 @@
       <c r="E59" t="s">
         <v>107</v>
       </c>
-      <c r="G59" t="s">
-        <v>594</v>
+      <c r="G59" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3443,8 +3487,8 @@
       <c r="E60" t="s">
         <v>109</v>
       </c>
-      <c r="G60" t="s">
-        <v>594</v>
+      <c r="G60" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3460,8 +3504,8 @@
       <c r="E61" t="s">
         <v>111</v>
       </c>
-      <c r="G61" t="s">
-        <v>594</v>
+      <c r="G61" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3477,8 +3521,8 @@
       <c r="E62" t="s">
         <v>113</v>
       </c>
-      <c r="G62" t="s">
-        <v>594</v>
+      <c r="G62" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3497,8 +3541,8 @@
       <c r="F63" t="s">
         <v>440</v>
       </c>
-      <c r="G63" t="s">
-        <v>594</v>
+      <c r="G63" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3514,8 +3558,8 @@
       <c r="E64" t="s">
         <v>116</v>
       </c>
-      <c r="G64" t="s">
-        <v>594</v>
+      <c r="G64" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3531,8 +3575,8 @@
       <c r="E65" t="s">
         <v>118</v>
       </c>
-      <c r="G65" t="s">
-        <v>594</v>
+      <c r="G65" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3548,8 +3592,8 @@
       <c r="E66" t="s">
         <v>120</v>
       </c>
-      <c r="G66" t="s">
-        <v>594</v>
+      <c r="G66" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3565,8 +3609,8 @@
       <c r="E67" t="s">
         <v>122</v>
       </c>
-      <c r="G67" t="s">
-        <v>594</v>
+      <c r="G67" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3582,8 +3626,8 @@
       <c r="E68" t="s">
         <v>124</v>
       </c>
-      <c r="G68" t="s">
-        <v>594</v>
+      <c r="G68" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3599,8 +3643,8 @@
       <c r="E69" t="s">
         <v>126</v>
       </c>
-      <c r="G69" t="s">
-        <v>594</v>
+      <c r="G69" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3616,8 +3660,8 @@
       <c r="E70" t="s">
         <v>128</v>
       </c>
-      <c r="G70" t="s">
-        <v>594</v>
+      <c r="G70" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3633,8 +3677,8 @@
       <c r="E71" t="s">
         <v>130</v>
       </c>
-      <c r="G71" t="s">
-        <v>594</v>
+      <c r="G71" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3650,8 +3694,8 @@
       <c r="E72" t="s">
         <v>132</v>
       </c>
-      <c r="G72" t="s">
-        <v>594</v>
+      <c r="G72" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3667,8 +3711,8 @@
       <c r="E73" t="s">
         <v>134</v>
       </c>
-      <c r="G73" t="s">
-        <v>594</v>
+      <c r="G73" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3684,8 +3728,8 @@
       <c r="E74" t="s">
         <v>136</v>
       </c>
-      <c r="G74" t="s">
-        <v>594</v>
+      <c r="G74" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3701,8 +3745,8 @@
       <c r="E75" t="s">
         <v>138</v>
       </c>
-      <c r="G75" t="s">
-        <v>594</v>
+      <c r="G75" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3718,8 +3762,8 @@
       <c r="E76" t="s">
         <v>140</v>
       </c>
-      <c r="G76" t="s">
-        <v>594</v>
+      <c r="G76" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3735,8 +3779,8 @@
       <c r="E77" t="s">
         <v>142</v>
       </c>
-      <c r="G77" t="s">
-        <v>594</v>
+      <c r="G77" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3752,8 +3796,8 @@
       <c r="E78" t="s">
         <v>144</v>
       </c>
-      <c r="G78" t="s">
-        <v>594</v>
+      <c r="G78" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3769,8 +3813,8 @@
       <c r="E79" t="s">
         <v>146</v>
       </c>
-      <c r="G79" t="s">
-        <v>594</v>
+      <c r="G79" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3786,8 +3830,8 @@
       <c r="E80" t="s">
         <v>148</v>
       </c>
-      <c r="G80" t="s">
-        <v>594</v>
+      <c r="G80" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3803,8 +3847,8 @@
       <c r="E81" t="s">
         <v>149</v>
       </c>
-      <c r="G81" t="s">
-        <v>594</v>
+      <c r="G81" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3820,8 +3864,8 @@
       <c r="E82" t="s">
         <v>151</v>
       </c>
-      <c r="G82" t="s">
-        <v>594</v>
+      <c r="G82" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3837,8 +3881,8 @@
       <c r="E83" t="s">
         <v>153</v>
       </c>
-      <c r="G83" t="s">
-        <v>594</v>
+      <c r="G83" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3854,8 +3898,8 @@
       <c r="E84" t="s">
         <v>155</v>
       </c>
-      <c r="G84" t="s">
-        <v>594</v>
+      <c r="G84" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3871,8 +3915,8 @@
       <c r="E85" t="s">
         <v>157</v>
       </c>
-      <c r="G85" t="s">
-        <v>594</v>
+      <c r="G85" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3888,8 +3932,8 @@
       <c r="E86" t="s">
         <v>159</v>
       </c>
-      <c r="G86" t="s">
-        <v>594</v>
+      <c r="G86" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3905,8 +3949,8 @@
       <c r="E87" t="s">
         <v>160</v>
       </c>
-      <c r="G87" t="s">
-        <v>594</v>
+      <c r="G87" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3922,8 +3966,8 @@
       <c r="E88" t="s">
         <v>161</v>
       </c>
-      <c r="G88" t="s">
-        <v>594</v>
+      <c r="G88" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3939,8 +3983,8 @@
       <c r="E89" t="s">
         <v>163</v>
       </c>
-      <c r="G89" t="s">
-        <v>594</v>
+      <c r="G89" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3956,8 +4000,8 @@
       <c r="E90" t="s">
         <v>165</v>
       </c>
-      <c r="G90" t="s">
-        <v>594</v>
+      <c r="G90" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3973,8 +4017,8 @@
       <c r="E91" t="s">
         <v>167</v>
       </c>
-      <c r="G91" t="s">
-        <v>594</v>
+      <c r="G91" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3990,8 +4034,8 @@
       <c r="E92" t="s">
         <v>169</v>
       </c>
-      <c r="G92" t="s">
-        <v>594</v>
+      <c r="G92" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4007,8 +4051,8 @@
       <c r="E93" t="s">
         <v>171</v>
       </c>
-      <c r="G93" t="s">
-        <v>594</v>
+      <c r="G93" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4024,8 +4068,8 @@
       <c r="E94" t="s">
         <v>173</v>
       </c>
-      <c r="G94" t="s">
-        <v>594</v>
+      <c r="G94" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4041,8 +4085,8 @@
       <c r="E95" t="s">
         <v>175</v>
       </c>
-      <c r="G95" t="s">
-        <v>594</v>
+      <c r="G95" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4058,8 +4102,8 @@
       <c r="E96" t="s">
         <v>176</v>
       </c>
-      <c r="G96" t="s">
-        <v>594</v>
+      <c r="G96" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4075,8 +4119,8 @@
       <c r="E97" t="s">
         <v>178</v>
       </c>
-      <c r="G97" t="s">
-        <v>594</v>
+      <c r="G97" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,8 +4136,8 @@
       <c r="E98" t="s">
         <v>180</v>
       </c>
-      <c r="G98" t="s">
-        <v>594</v>
+      <c r="G98" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4109,8 +4153,8 @@
       <c r="E99" t="s">
         <v>182</v>
       </c>
-      <c r="G99" t="s">
-        <v>594</v>
+      <c r="G99" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4126,8 +4170,8 @@
       <c r="E100" t="s">
         <v>184</v>
       </c>
-      <c r="G100" t="s">
-        <v>594</v>
+      <c r="G100" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4143,8 +4187,8 @@
       <c r="E101" t="s">
         <v>186</v>
       </c>
-      <c r="G101" t="s">
-        <v>594</v>
+      <c r="G101" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4160,8 +4204,8 @@
       <c r="E102" t="s">
         <v>188</v>
       </c>
-      <c r="G102" t="s">
-        <v>594</v>
+      <c r="G102" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4177,8 +4221,8 @@
       <c r="E103" t="s">
         <v>189</v>
       </c>
-      <c r="G103" t="s">
-        <v>594</v>
+      <c r="G103" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4194,8 +4238,8 @@
       <c r="E104" t="s">
         <v>191</v>
       </c>
-      <c r="G104" t="s">
-        <v>594</v>
+      <c r="G104" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4214,8 +4258,8 @@
       <c r="F105" t="s">
         <v>309</v>
       </c>
-      <c r="G105" t="s">
-        <v>594</v>
+      <c r="G105" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4234,8 +4278,8 @@
       <c r="F106" t="s">
         <v>310</v>
       </c>
-      <c r="G106" t="s">
-        <v>594</v>
+      <c r="G106" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4251,8 +4295,8 @@
       <c r="E107" t="s">
         <v>197</v>
       </c>
-      <c r="G107" t="s">
-        <v>594</v>
+      <c r="G107" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4268,8 +4312,8 @@
       <c r="E108" t="s">
         <v>199</v>
       </c>
-      <c r="G108" t="s">
-        <v>594</v>
+      <c r="G108" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4285,8 +4329,8 @@
       <c r="E109" t="s">
         <v>201</v>
       </c>
-      <c r="G109" t="s">
-        <v>594</v>
+      <c r="G109" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4302,8 +4346,8 @@
       <c r="E110" t="s">
         <v>203</v>
       </c>
-      <c r="G110" t="s">
-        <v>594</v>
+      <c r="G110" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4319,8 +4363,8 @@
       <c r="E111" t="s">
         <v>204</v>
       </c>
-      <c r="G111" t="s">
-        <v>594</v>
+      <c r="G111" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4336,8 +4380,8 @@
       <c r="E112" t="s">
         <v>206</v>
       </c>
-      <c r="G112" t="s">
-        <v>594</v>
+      <c r="G112" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4353,8 +4397,8 @@
       <c r="E113" t="s">
         <v>208</v>
       </c>
-      <c r="G113" t="s">
-        <v>594</v>
+      <c r="G113" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4370,8 +4414,8 @@
       <c r="E114" t="s">
         <v>210</v>
       </c>
-      <c r="G114" t="s">
-        <v>594</v>
+      <c r="G114" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4387,8 +4431,8 @@
       <c r="E115" t="s">
         <v>212</v>
       </c>
-      <c r="G115" t="s">
-        <v>594</v>
+      <c r="G115" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4404,8 +4448,8 @@
       <c r="E116" t="s">
         <v>214</v>
       </c>
-      <c r="G116" t="s">
-        <v>594</v>
+      <c r="G116" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4421,8 +4465,8 @@
       <c r="E117" t="s">
         <v>216</v>
       </c>
-      <c r="G117" t="s">
-        <v>594</v>
+      <c r="G117" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4438,8 +4482,8 @@
       <c r="E118" t="s">
         <v>218</v>
       </c>
-      <c r="G118" t="s">
-        <v>594</v>
+      <c r="G118" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4455,8 +4499,8 @@
       <c r="E119" t="s">
         <v>220</v>
       </c>
-      <c r="G119" t="s">
-        <v>594</v>
+      <c r="G119" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -4475,8 +4519,8 @@
       <c r="F120" t="s">
         <v>311</v>
       </c>
-      <c r="G120" t="s">
-        <v>594</v>
+      <c r="G120" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -4492,8 +4536,8 @@
       <c r="E121" t="s">
         <v>223</v>
       </c>
-      <c r="G121" t="s">
-        <v>594</v>
+      <c r="G121" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4512,8 +4556,8 @@
       <c r="F122" t="s">
         <v>312</v>
       </c>
-      <c r="G122" t="s">
-        <v>594</v>
+      <c r="G122" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4529,8 +4573,8 @@
       <c r="E123" t="s">
         <v>227</v>
       </c>
-      <c r="G123" t="s">
-        <v>594</v>
+      <c r="G123" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4546,8 +4590,8 @@
       <c r="E124" t="s">
         <v>229</v>
       </c>
-      <c r="G124" t="s">
-        <v>594</v>
+      <c r="G124" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4563,8 +4607,8 @@
       <c r="E125" t="s">
         <v>231</v>
       </c>
-      <c r="G125" t="s">
-        <v>594</v>
+      <c r="G125" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -4580,8 +4624,8 @@
       <c r="E126" t="s">
         <v>233</v>
       </c>
-      <c r="G126" t="s">
-        <v>594</v>
+      <c r="G126" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -4597,8 +4641,8 @@
       <c r="E127" t="s">
         <v>235</v>
       </c>
-      <c r="G127" t="s">
-        <v>594</v>
+      <c r="G127" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4614,8 +4658,8 @@
       <c r="E128" t="s">
         <v>237</v>
       </c>
-      <c r="G128" t="s">
-        <v>594</v>
+      <c r="G128" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4631,8 +4675,8 @@
       <c r="E129" t="s">
         <v>239</v>
       </c>
-      <c r="G129" t="s">
-        <v>594</v>
+      <c r="G129" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -4648,8 +4692,8 @@
       <c r="E130" t="s">
         <v>241</v>
       </c>
-      <c r="G130" t="s">
-        <v>594</v>
+      <c r="G130" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4665,8 +4709,8 @@
       <c r="E131" t="s">
         <v>243</v>
       </c>
-      <c r="G131" t="s">
-        <v>594</v>
+      <c r="G131" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4685,8 +4729,8 @@
       <c r="F132" t="s">
         <v>313</v>
       </c>
-      <c r="G132" t="s">
-        <v>594</v>
+      <c r="G132" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4702,8 +4746,8 @@
       <c r="E133" t="s">
         <v>247</v>
       </c>
-      <c r="G133" t="s">
-        <v>594</v>
+      <c r="G133" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4719,8 +4763,8 @@
       <c r="E134" t="s">
         <v>249</v>
       </c>
-      <c r="G134" t="s">
-        <v>594</v>
+      <c r="G134" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4736,8 +4780,8 @@
       <c r="E135" t="s">
         <v>251</v>
       </c>
-      <c r="G135" t="s">
-        <v>594</v>
+      <c r="G135" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4753,8 +4797,8 @@
       <c r="E136" t="s">
         <v>253</v>
       </c>
-      <c r="G136" t="s">
-        <v>594</v>
+      <c r="G136" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4770,8 +4814,8 @@
       <c r="E137" t="s">
         <v>255</v>
       </c>
-      <c r="G137" t="s">
-        <v>594</v>
+      <c r="G137" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4787,8 +4831,8 @@
       <c r="E138" t="s">
         <v>257</v>
       </c>
-      <c r="G138" t="s">
-        <v>594</v>
+      <c r="G138" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4804,8 +4848,8 @@
       <c r="E139" t="s">
         <v>259</v>
       </c>
-      <c r="G139" t="s">
-        <v>594</v>
+      <c r="G139" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -4821,8 +4865,8 @@
       <c r="E140" t="s">
         <v>261</v>
       </c>
-      <c r="G140" t="s">
-        <v>594</v>
+      <c r="G140" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -4838,8 +4882,8 @@
       <c r="E141" t="s">
         <v>263</v>
       </c>
-      <c r="G141" t="s">
-        <v>594</v>
+      <c r="G141" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4855,8 +4899,8 @@
       <c r="E142" t="s">
         <v>265</v>
       </c>
-      <c r="G142" t="s">
-        <v>594</v>
+      <c r="G142" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -4872,8 +4916,8 @@
       <c r="E143" t="s">
         <v>267</v>
       </c>
-      <c r="G143" t="s">
-        <v>594</v>
+      <c r="G143" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -4889,8 +4933,8 @@
       <c r="E144" t="s">
         <v>269</v>
       </c>
-      <c r="G144" t="s">
-        <v>594</v>
+      <c r="G144" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -4906,8 +4950,8 @@
       <c r="E145" t="s">
         <v>271</v>
       </c>
-      <c r="G145" t="s">
-        <v>594</v>
+      <c r="G145" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4923,8 +4967,8 @@
       <c r="E146" t="s">
         <v>273</v>
       </c>
-      <c r="G146" t="s">
-        <v>594</v>
+      <c r="G146" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -4940,8 +4984,8 @@
       <c r="E147" t="s">
         <v>275</v>
       </c>
-      <c r="G147" t="s">
-        <v>594</v>
+      <c r="G147" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -4957,8 +5001,8 @@
       <c r="E148" t="s">
         <v>277</v>
       </c>
-      <c r="G148" t="s">
-        <v>594</v>
+      <c r="G148" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -4974,8 +5018,8 @@
       <c r="E149" t="s">
         <v>279</v>
       </c>
-      <c r="G149" t="s">
-        <v>594</v>
+      <c r="G149" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -4991,8 +5035,8 @@
       <c r="E150" t="s">
         <v>280</v>
       </c>
-      <c r="G150" t="s">
-        <v>594</v>
+      <c r="G150" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -5008,8 +5052,8 @@
       <c r="E151" t="s">
         <v>282</v>
       </c>
-      <c r="G151" t="s">
-        <v>594</v>
+      <c r="G151" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -5025,8 +5069,8 @@
       <c r="E152" t="s">
         <v>284</v>
       </c>
-      <c r="G152" t="s">
-        <v>594</v>
+      <c r="G152" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5042,8 +5086,8 @@
       <c r="E153" t="s">
         <v>285</v>
       </c>
-      <c r="G153" t="s">
-        <v>594</v>
+      <c r="G153" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -5059,8 +5103,8 @@
       <c r="E154" t="s">
         <v>287</v>
       </c>
-      <c r="G154" t="s">
-        <v>594</v>
+      <c r="G154" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -5076,8 +5120,8 @@
       <c r="E155" t="s">
         <v>289</v>
       </c>
-      <c r="G155" t="s">
-        <v>594</v>
+      <c r="G155" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5093,8 +5137,8 @@
       <c r="E156" t="s">
         <v>291</v>
       </c>
-      <c r="G156" t="s">
-        <v>594</v>
+      <c r="G156" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -5113,8 +5157,8 @@
       <c r="F157" t="s">
         <v>314</v>
       </c>
-      <c r="G157" t="s">
-        <v>594</v>
+      <c r="G157" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5130,8 +5174,8 @@
       <c r="E158" t="s">
         <v>294</v>
       </c>
-      <c r="G158" t="s">
-        <v>594</v>
+      <c r="G158" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5150,8 +5194,8 @@
       <c r="F159" t="s">
         <v>315</v>
       </c>
-      <c r="G159" t="s">
-        <v>594</v>
+      <c r="G159" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -5167,8 +5211,8 @@
       <c r="E160" t="s">
         <v>298</v>
       </c>
-      <c r="G160" t="s">
-        <v>594</v>
+      <c r="G160" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5184,8 +5228,8 @@
       <c r="E161" t="s">
         <v>300</v>
       </c>
-      <c r="G161" t="s">
-        <v>594</v>
+      <c r="G161" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5204,8 +5248,8 @@
       <c r="F162" t="s">
         <v>316</v>
       </c>
-      <c r="G162" t="s">
-        <v>594</v>
+      <c r="G162" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -5221,6 +5265,7 @@
       <c r="E163" s="3" t="s">
         <v>476</v>
       </c>
+      <c r="G163" s="4"/>
     </row>
     <row r="164" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
@@ -5235,6 +5280,7 @@
       <c r="E164" s="3" t="s">
         <v>504</v>
       </c>
+      <c r="G164" s="4"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
@@ -5244,16 +5290,16 @@
         <v>474</v>
       </c>
       <c r="C165" t="s">
+        <v>582</v>
+      </c>
+      <c r="E165" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="E165" s="3" t="s">
+      <c r="F165" t="s">
         <v>584</v>
       </c>
-      <c r="F165" t="s">
-        <v>585</v>
-      </c>
-      <c r="G165" t="s">
-        <v>594</v>
+      <c r="G165" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5264,16 +5310,16 @@
         <v>474</v>
       </c>
       <c r="C166" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>289</v>
       </c>
       <c r="F166" t="s">
-        <v>587</v>
-      </c>
-      <c r="G166" t="s">
-        <v>594</v>
+        <v>586</v>
+      </c>
+      <c r="G166" s="4" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -5284,14 +5330,15 @@
         <v>474</v>
       </c>
       <c r="C167" t="s">
+        <v>587</v>
+      </c>
+      <c r="E167" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="E167" s="3" t="s">
+      <c r="F167" t="s">
         <v>589</v>
       </c>
-      <c r="F167" t="s">
-        <v>590</v>
-      </c>
+      <c r="G167" s="4"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
@@ -5306,6 +5353,7 @@
       <c r="E168" s="1" t="s">
         <v>523</v>
       </c>
+      <c r="G168" s="4"/>
     </row>
     <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
@@ -5323,6 +5371,7 @@
       <c r="F169" t="s">
         <v>524</v>
       </c>
+      <c r="G169" s="4"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
@@ -5337,6 +5386,7 @@
       <c r="E170" s="3" t="s">
         <v>522</v>
       </c>
+      <c r="G170" s="4"/>
     </row>
     <row r="171" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
@@ -5351,6 +5401,7 @@
       <c r="E171" s="3" t="s">
         <v>470</v>
       </c>
+      <c r="G171" s="4"/>
     </row>
     <row r="172" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
@@ -5365,6 +5416,7 @@
       <c r="E172" s="3" t="s">
         <v>473</v>
       </c>
+      <c r="G172" s="4"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
@@ -5373,155 +5425,164 @@
       <c r="B173" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G173" s="4"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B174" t="s">
-        <v>576</v>
+        <v>644</v>
       </c>
       <c r="C174" t="s">
-        <v>577</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>579</v>
+        <v>638</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>636</v>
       </c>
       <c r="F174" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>639</v>
+      </c>
+      <c r="G174" s="4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B175" t="s">
+        <v>644</v>
+      </c>
+      <c r="C175" t="s">
+        <v>637</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="F175" t="s">
+        <v>640</v>
+      </c>
+      <c r="G175" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B176" t="s">
+        <v>645</v>
+      </c>
+      <c r="C176" t="s">
         <v>576</v>
       </c>
-      <c r="C175" t="s">
+      <c r="E176" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="E175" s="2" t="s">
+      <c r="F176" t="s">
         <v>581</v>
       </c>
-      <c r="F175" t="s">
+      <c r="G176" s="4"/>
+    </row>
+    <row r="177" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B177" t="s">
+        <v>645</v>
+      </c>
+      <c r="C177" t="s">
+        <v>577</v>
+      </c>
+      <c r="E177" s="2" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="F177" t="s">
+        <v>579</v>
+      </c>
+      <c r="G177" s="4"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>355</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B178" t="s">
         <v>359</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C178" t="s">
         <v>360</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E178" t="s">
         <v>319</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F178" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>355</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B179" t="s">
         <v>359</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C179" t="s">
         <v>361</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E179" t="s">
         <v>535</v>
       </c>
-      <c r="F177" t="s">
+      <c r="F179" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>356</v>
-      </c>
-      <c r="B178" t="s">
-        <v>58</v>
-      </c>
-      <c r="C178" t="s">
-        <v>455</v>
-      </c>
-      <c r="E178" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>356</v>
-      </c>
-      <c r="B179" t="s">
-        <v>58</v>
-      </c>
-      <c r="C179" t="s">
-        <v>456</v>
-      </c>
-      <c r="E179" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
       <c r="B180" t="s">
-        <v>321</v>
+        <v>58</v>
       </c>
       <c r="C180" t="s">
-        <v>321</v>
+        <v>455</v>
       </c>
       <c r="E180" t="s">
-        <v>534</v>
-      </c>
-      <c r="F180" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>356</v>
       </c>
       <c r="B181" t="s">
-        <v>358</v>
+        <v>58</v>
       </c>
       <c r="C181" t="s">
-        <v>322</v>
+        <v>456</v>
       </c>
       <c r="E181" t="s">
-        <v>323</v>
-      </c>
-      <c r="F181" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>356</v>
       </c>
       <c r="B182" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="C182" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E182" t="s">
-        <v>325</v>
+        <v>534</v>
       </c>
       <c r="F182" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>356</v>
       </c>
@@ -5529,16 +5590,16 @@
         <v>358</v>
       </c>
       <c r="C183" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E183" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F183" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>356</v>
       </c>
@@ -5546,16 +5607,16 @@
         <v>358</v>
       </c>
       <c r="C184" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E184" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F184" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>356</v>
       </c>
@@ -5563,16 +5624,16 @@
         <v>358</v>
       </c>
       <c r="C185" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E185" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F185" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>356</v>
       </c>
@@ -5580,16 +5641,16 @@
         <v>358</v>
       </c>
       <c r="C186" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E186" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F186" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>356</v>
       </c>
@@ -5597,16 +5658,16 @@
         <v>358</v>
       </c>
       <c r="C187" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E187" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F187" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>356</v>
       </c>
@@ -5614,13 +5675,16 @@
         <v>358</v>
       </c>
       <c r="C188" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E188" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="F188" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>356</v>
       </c>
@@ -5628,47 +5692,44 @@
         <v>358</v>
       </c>
       <c r="C189" t="s">
+        <v>334</v>
+      </c>
+      <c r="E189" t="s">
+        <v>335</v>
+      </c>
+      <c r="F189" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>356</v>
+      </c>
+      <c r="B190" t="s">
+        <v>358</v>
+      </c>
+      <c r="C190" t="s">
+        <v>336</v>
+      </c>
+      <c r="E190" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>356</v>
+      </c>
+      <c r="B191" t="s">
+        <v>358</v>
+      </c>
+      <c r="C191" t="s">
         <v>338</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E191" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>478</v>
-      </c>
-      <c r="B190" t="s">
-        <v>1</v>
-      </c>
-      <c r="C190" t="s">
-        <v>2</v>
-      </c>
-      <c r="E190" t="s">
-        <v>340</v>
-      </c>
-      <c r="F190" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>478</v>
-      </c>
-      <c r="B191" t="s">
-        <v>1</v>
-      </c>
-      <c r="C191" t="s">
-        <v>362</v>
-      </c>
-      <c r="E191" t="s">
-        <v>341</v>
-      </c>
-      <c r="F191" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>478</v>
       </c>
@@ -5676,13 +5737,13 @@
         <v>1</v>
       </c>
       <c r="C192" t="s">
-        <v>215</v>
+        <v>2</v>
       </c>
       <c r="E192" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F192" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -5693,13 +5754,13 @@
         <v>1</v>
       </c>
       <c r="C193" t="s">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="E193" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F193" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -5710,13 +5771,13 @@
         <v>1</v>
       </c>
       <c r="C194" t="s">
-        <v>363</v>
+        <v>215</v>
       </c>
       <c r="E194" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F194" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -5727,47 +5788,47 @@
         <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>364</v>
+        <v>22</v>
       </c>
       <c r="E195" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F195" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B196" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>112</v>
+        <v>363</v>
       </c>
       <c r="E196" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="F196" t="s">
-        <v>388</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B197" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C197" t="s">
-        <v>54</v>
+        <v>364</v>
       </c>
       <c r="E197" t="s">
-        <v>389</v>
+        <v>345</v>
       </c>
       <c r="F197" t="s">
-        <v>390</v>
+        <v>18</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -5778,13 +5839,13 @@
         <v>303</v>
       </c>
       <c r="C198" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E198" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F198" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -5795,13 +5856,13 @@
         <v>303</v>
       </c>
       <c r="C199" t="s">
-        <v>426</v>
+        <v>54</v>
       </c>
       <c r="E199" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F199" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -5812,13 +5873,13 @@
         <v>303</v>
       </c>
       <c r="C200" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E200" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F200" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -5829,13 +5890,13 @@
         <v>303</v>
       </c>
       <c r="C201" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E201" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F201" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -5846,13 +5907,13 @@
         <v>303</v>
       </c>
       <c r="C202" t="s">
-        <v>427</v>
+        <v>58</v>
       </c>
       <c r="E202" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F202" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -5863,13 +5924,13 @@
         <v>303</v>
       </c>
       <c r="C203" t="s">
-        <v>174</v>
+        <v>428</v>
       </c>
       <c r="E203" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F203" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -5880,13 +5941,13 @@
         <v>303</v>
       </c>
       <c r="C204" t="s">
-        <v>84</v>
+        <v>427</v>
       </c>
       <c r="E204" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F204" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -5897,13 +5958,13 @@
         <v>303</v>
       </c>
       <c r="C205" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="E205" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F205" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5911,16 +5972,16 @@
         <v>357</v>
       </c>
       <c r="B206" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C206" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E206" t="s">
-        <v>365</v>
+        <v>403</v>
       </c>
       <c r="F206" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -5928,16 +5989,16 @@
         <v>357</v>
       </c>
       <c r="B207" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C207" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="E207" t="s">
-        <v>367</v>
+        <v>405</v>
       </c>
       <c r="F207" t="s">
-        <v>368</v>
+        <v>406</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -5948,13 +6009,13 @@
         <v>304</v>
       </c>
       <c r="C208" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E208" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F208" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -5965,13 +6026,13 @@
         <v>304</v>
       </c>
       <c r="C209" t="s">
-        <v>427</v>
+        <v>54</v>
       </c>
       <c r="E209" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F209" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -5982,13 +6043,13 @@
         <v>304</v>
       </c>
       <c r="C210" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="E210" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F210" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -5999,13 +6060,13 @@
         <v>304</v>
       </c>
       <c r="C211" t="s">
-        <v>141</v>
+        <v>427</v>
       </c>
       <c r="E211" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F211" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -6016,13 +6077,13 @@
         <v>304</v>
       </c>
       <c r="C212" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="E212" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F212" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -6033,13 +6094,13 @@
         <v>304</v>
       </c>
       <c r="C213" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E213" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F213" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -6050,13 +6111,13 @@
         <v>304</v>
       </c>
       <c r="C214" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="E214" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F214" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -6067,13 +6128,13 @@
         <v>304</v>
       </c>
       <c r="C215" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E215" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F215" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -6084,13 +6145,13 @@
         <v>304</v>
       </c>
       <c r="C216" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E216" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F216" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
@@ -6098,16 +6159,16 @@
         <v>357</v>
       </c>
       <c r="B217" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C217" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E217" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="F217" t="s">
-        <v>439</v>
+        <v>384</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
@@ -6115,16 +6176,16 @@
         <v>357</v>
       </c>
       <c r="B218" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C218" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="E218" t="s">
-        <v>347</v>
+        <v>385</v>
       </c>
       <c r="F218" t="s">
-        <v>438</v>
+        <v>386</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -6135,13 +6196,13 @@
         <v>305</v>
       </c>
       <c r="C219" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="E219" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F219" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -6152,13 +6213,13 @@
         <v>305</v>
       </c>
       <c r="C220" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="E220" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F220" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -6169,13 +6230,13 @@
         <v>305</v>
       </c>
       <c r="C221" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E221" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F221" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -6186,13 +6247,13 @@
         <v>305</v>
       </c>
       <c r="C222" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E222" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F222" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -6203,13 +6264,13 @@
         <v>305</v>
       </c>
       <c r="C223" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="E223" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F223" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -6220,13 +6281,13 @@
         <v>305</v>
       </c>
       <c r="C224" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E224" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F224" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -6237,47 +6298,47 @@
         <v>305</v>
       </c>
       <c r="C225" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="E225" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F225" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B226" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C226" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="E226" t="s">
-        <v>409</v>
+        <v>353</v>
       </c>
       <c r="F226" t="s">
-        <v>410</v>
+        <v>432</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B227" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C227" t="s">
-        <v>205</v>
+        <v>262</v>
       </c>
       <c r="E227" t="s">
-        <v>411</v>
+        <v>354</v>
       </c>
       <c r="F227" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -6288,13 +6349,13 @@
         <v>425</v>
       </c>
       <c r="C228" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E228" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F228" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -6305,13 +6366,13 @@
         <v>425</v>
       </c>
       <c r="C229" t="s">
-        <v>283</v>
+        <v>205</v>
       </c>
       <c r="E229" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F229" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -6322,13 +6383,13 @@
         <v>425</v>
       </c>
       <c r="C230" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E230" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F230" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -6339,13 +6400,13 @@
         <v>425</v>
       </c>
       <c r="C231" t="s">
-        <v>430</v>
+        <v>283</v>
       </c>
       <c r="E231" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F231" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
@@ -6353,50 +6414,50 @@
         <v>423</v>
       </c>
       <c r="B232" t="s">
-        <v>306</v>
+        <v>425</v>
       </c>
       <c r="C232" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="E232" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F232" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B233" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C233" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E233" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="F233" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B234" t="s">
-        <v>442</v>
+        <v>306</v>
       </c>
       <c r="C234" t="s">
-        <v>443</v>
+        <v>306</v>
       </c>
       <c r="E234" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="F234" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -6404,16 +6465,16 @@
         <v>424</v>
       </c>
       <c r="B235" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C235" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="E235" t="s">
-        <v>446</v>
+        <v>407</v>
       </c>
       <c r="F235" t="s">
-        <v>447</v>
+        <v>408</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
@@ -6424,13 +6485,13 @@
         <v>442</v>
       </c>
       <c r="C236" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E236" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F236" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -6441,115 +6502,109 @@
         <v>442</v>
       </c>
       <c r="C237" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E237" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="F237" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>424</v>
+      </c>
+      <c r="B238" t="s">
+        <v>442</v>
+      </c>
+      <c r="C238" t="s">
+        <v>449</v>
+      </c>
+      <c r="E238" t="s">
+        <v>450</v>
+      </c>
+      <c r="F238" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>424</v>
+      </c>
+      <c r="B239" t="s">
+        <v>442</v>
+      </c>
+      <c r="C239" t="s">
+        <v>452</v>
+      </c>
+      <c r="E239" t="s">
+        <v>453</v>
+      </c>
+      <c r="F239" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
         <v>464</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B240" t="s">
         <v>462</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C240" t="s">
         <v>463</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E240" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B241" t="s">
         <v>462</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C241" t="s">
         <v>468</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E241" t="s">
         <v>562</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B240" t="s">
-        <v>481</v>
-      </c>
-      <c r="C240" t="s">
-        <v>482</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F240" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>484</v>
-      </c>
-      <c r="B241" t="s">
-        <v>481</v>
-      </c>
-      <c r="C241" t="s">
-        <v>483</v>
-      </c>
-      <c r="E241" t="s">
-        <v>496</v>
-      </c>
-      <c r="F241" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
       <c r="B242" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="C242" t="s">
-        <v>627</v>
-      </c>
-      <c r="E242" t="s">
-        <v>467</v>
+        <v>482</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>495</v>
       </c>
       <c r="F242" t="s">
-        <v>612</v>
-      </c>
-      <c r="G242" t="s">
-        <v>626</v>
+        <v>485</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>466</v>
+      <c r="A243" t="s">
+        <v>484</v>
       </c>
       <c r="B243" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="C243" t="s">
-        <v>628</v>
+        <v>483</v>
       </c>
       <c r="E243" t="s">
-        <v>614</v>
+        <v>496</v>
       </c>
       <c r="F243" t="s">
-        <v>613</v>
-      </c>
-      <c r="G243" t="s">
-        <v>626</v>
+        <v>486</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -6560,16 +6615,16 @@
         <v>462</v>
       </c>
       <c r="C244" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E244" t="s">
-        <v>615</v>
+        <v>467</v>
       </c>
       <c r="F244" t="s">
-        <v>616</v>
-      </c>
-      <c r="G244" t="s">
-        <v>626</v>
+        <v>611</v>
+      </c>
+      <c r="G244" s="4" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -6580,16 +6635,16 @@
         <v>462</v>
       </c>
       <c r="C245" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E245" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="F245" t="s">
-        <v>618</v>
-      </c>
-      <c r="G245" t="s">
-        <v>626</v>
+        <v>612</v>
+      </c>
+      <c r="G245" s="4" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -6600,16 +6655,16 @@
         <v>462</v>
       </c>
       <c r="C246" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E246" t="s">
-        <v>563</v>
+        <v>614</v>
       </c>
       <c r="F246" t="s">
-        <v>619</v>
-      </c>
-      <c r="G246" t="s">
-        <v>626</v>
+        <v>615</v>
+      </c>
+      <c r="G246" s="4" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -6620,16 +6675,16 @@
         <v>462</v>
       </c>
       <c r="C247" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E247" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="F247" t="s">
-        <v>621</v>
-      </c>
-      <c r="G247" t="s">
-        <v>626</v>
+        <v>617</v>
+      </c>
+      <c r="G247" s="4" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -6640,16 +6695,16 @@
         <v>462</v>
       </c>
       <c r="C248" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E248" t="s">
-        <v>622</v>
+        <v>563</v>
       </c>
       <c r="F248" t="s">
-        <v>623</v>
-      </c>
-      <c r="G248" t="s">
-        <v>626</v>
+        <v>618</v>
+      </c>
+      <c r="G248" s="4" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -6660,16 +6715,16 @@
         <v>462</v>
       </c>
       <c r="C249" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E249" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="F249" t="s">
+        <v>620</v>
+      </c>
+      <c r="G249" s="4" t="s">
         <v>625</v>
-      </c>
-      <c r="G249" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -6677,206 +6732,223 @@
         <v>466</v>
       </c>
       <c r="B250" t="s">
+        <v>462</v>
+      </c>
+      <c r="C250" t="s">
+        <v>632</v>
+      </c>
+      <c r="E250" t="s">
+        <v>621</v>
+      </c>
+      <c r="F250" t="s">
+        <v>622</v>
+      </c>
+      <c r="G250" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B251" t="s">
+        <v>462</v>
+      </c>
+      <c r="C251" t="s">
+        <v>633</v>
+      </c>
+      <c r="E251" t="s">
+        <v>623</v>
+      </c>
+      <c r="F251" t="s">
+        <v>624</v>
+      </c>
+      <c r="G251" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B252" t="s">
+        <v>646</v>
+      </c>
+      <c r="C252" t="s">
+        <v>634</v>
+      </c>
+      <c r="E252" t="s">
         <v>635</v>
       </c>
-      <c r="C250" t="s">
-        <v>636</v>
-      </c>
-      <c r="E250" t="s">
-        <v>637</v>
-      </c>
-      <c r="F250" t="s">
+      <c r="F252" t="s">
+        <v>624</v>
+      </c>
+      <c r="G252" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="G250" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B251" t="s">
-        <v>480</v>
-      </c>
-      <c r="C251" t="s">
-        <v>488</v>
-      </c>
-      <c r="E251" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F251" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B252" t="s">
-        <v>480</v>
-      </c>
-      <c r="C252" t="s">
-        <v>489</v>
-      </c>
-      <c r="E252" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F252" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B253" t="s">
-        <v>480</v>
+        <v>646</v>
       </c>
       <c r="C253" t="s">
-        <v>491</v>
-      </c>
-      <c r="E253" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+      <c r="E253" t="s">
+        <v>650</v>
+      </c>
+      <c r="F253" t="s">
+        <v>649</v>
+      </c>
+      <c r="G253" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B254" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C254" t="s">
-        <v>482</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
+      </c>
+      <c r="E254" s="3" t="s">
+        <v>497</v>
       </c>
       <c r="F254" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+      <c r="G254" s="4"/>
+    </row>
+    <row r="255" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B255" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C255" t="s">
-        <v>483</v>
-      </c>
-      <c r="E255" t="s">
-        <v>494</v>
+        <v>489</v>
+      </c>
+      <c r="E255" s="3" t="s">
+        <v>498</v>
       </c>
       <c r="F255" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+      <c r="G255" s="4"/>
+    </row>
+    <row r="256" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B256" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="C256" t="s">
-        <v>500</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F256" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+        <v>491</v>
+      </c>
+      <c r="E256" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="G256" s="4"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B257" t="s">
-        <v>575</v>
+        <v>481</v>
       </c>
       <c r="C257" t="s">
-        <v>572</v>
+        <v>482</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>574</v>
+        <v>493</v>
       </c>
       <c r="F257" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+      <c r="G257" s="4"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B258" t="s">
-        <v>568</v>
+        <v>481</v>
       </c>
       <c r="C258" t="s">
-        <v>569</v>
-      </c>
-      <c r="E258" s="3" t="s">
-        <v>570</v>
+        <v>483</v>
+      </c>
+      <c r="E258" t="s">
+        <v>494</v>
       </c>
       <c r="F258" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+      <c r="G258" s="4"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B259" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C259" t="s">
-        <v>508</v>
-      </c>
-      <c r="E259" s="2" t="s">
-        <v>561</v>
+        <v>500</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="F259" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="G259" s="4"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B260" t="s">
-        <v>506</v>
+        <v>575</v>
       </c>
       <c r="C260" t="s">
-        <v>509</v>
+        <v>572</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F260" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+      <c r="F260" t="s">
+        <v>573</v>
+      </c>
+      <c r="G260" s="4"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B261" t="s">
-        <v>505</v>
+        <v>568</v>
       </c>
       <c r="C261" t="s">
-        <v>511</v>
+        <v>569</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="F261" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+      <c r="G261" s="4"/>
+    </row>
+    <row r="262" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>479</v>
       </c>
@@ -6884,33 +6956,35 @@
         <v>506</v>
       </c>
       <c r="C262" t="s">
-        <v>513</v>
-      </c>
-      <c r="E262" s="1" t="s">
-        <v>560</v>
+        <v>508</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>561</v>
       </c>
       <c r="F262" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+      <c r="G262" s="4"/>
+    </row>
+    <row r="263" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B263" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C263" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="F263" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+      <c r="F263" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="G263" s="4"/>
+    </row>
+    <row r="264" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>479</v>
       </c>
@@ -6918,33 +6992,35 @@
         <v>505</v>
       </c>
       <c r="C264" t="s">
-        <v>525</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>518</v>
+        <v>511</v>
+      </c>
+      <c r="E264" s="3" t="s">
+        <v>566</v>
       </c>
       <c r="F264" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+      <c r="G264" s="4"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B265" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C265" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>518</v>
+        <v>560</v>
       </c>
       <c r="F265" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="G265" s="4"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>479</v>
       </c>
@@ -6952,31 +7028,87 @@
         <v>505</v>
       </c>
       <c r="C266" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>597</v>
+        <v>516</v>
       </c>
       <c r="F266" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="G266" s="4"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B267" t="s">
+        <v>505</v>
+      </c>
+      <c r="C267" t="s">
+        <v>525</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F267" t="s">
+        <v>527</v>
+      </c>
+      <c r="G267" s="4"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B268" t="s">
+        <v>505</v>
+      </c>
+      <c r="C268" t="s">
+        <v>517</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F268" t="s">
+        <v>528</v>
+      </c>
+      <c r="G268" s="4"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B269" t="s">
+        <v>505</v>
+      </c>
+      <c r="C269" t="s">
+        <v>529</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="F269" t="s">
+        <v>530</v>
+      </c>
+      <c r="G269" s="4"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B270" t="s">
         <v>506</v>
       </c>
-      <c r="C267" t="s">
+      <c r="C270" t="s">
         <v>531</v>
       </c>
-      <c r="E267" s="1" t="s">
+      <c r="E270" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F267" t="s">
+      <c r="F270" t="s">
         <v>532</v>
       </c>
+      <c r="G270" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add sub-template snippets - close https://github.com/2sic/2sxc/issues/1098
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="661">
   <si>
     <t>set</t>
   </si>
@@ -2036,6 +2036,40 @@
   </si>
   <si>
     <t>&lt;script type="text/javascript" src="/desktopmodules/tosic_sexycontent/js/angularjs/angular.min.js" data-enableoptimizations="101"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>Render separate cshtml (sub-template)</t>
+  </si>
+  <si>
+    <t>Render separate cshtml with params (sub-template)</t>
+  </si>
+  <si>
+    <t>Create instance of CSHTML with library functions</t>
+  </si>
+  <si>
+    <t>In a sub-template, access parameter given in</t>
+  </si>
+  <si>
+    <t>Render sub-template</t>
+  </si>
+  <si>
+    <t>Render sub-template w/params</t>
+  </si>
+  <si>
+    <t>@{
+    var lib = CreateInstance("_${1:library}.cshtml"); 
+}</t>
+  </si>
+  <si>
+    <t>@{
+    var ${2:post} = PageData["${1:Post}"];
+}</t>
+  </si>
+  <si>
+    <t>@RenderPage("_${1:list-item}.cshtml", new { ${2:Post} = ${3:post} })</t>
+  </si>
+  <si>
+    <t>@RenderPage("_${1:list-item}.cshtml")</t>
   </si>
 </sst>
 </file>
@@ -2099,8 +2133,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G270" totalsRowShown="0">
-  <autoFilter ref="A1:G270"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G274" totalsRowShown="0">
+  <autoFilter ref="A1:G274"/>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2377,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G270"/>
+  <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="G253" sqref="G253"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5504,99 +5538,109 @@
       <c r="G177" s="4"/>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>355</v>
+      <c r="A178" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B178" t="s">
-        <v>359</v>
+        <v>460</v>
       </c>
       <c r="C178" t="s">
-        <v>360</v>
-      </c>
-      <c r="E178" t="s">
-        <v>319</v>
+        <v>655</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>660</v>
       </c>
       <c r="F178" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>355</v>
+        <v>651</v>
+      </c>
+      <c r="G178" s="4"/>
+    </row>
+    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B179" t="s">
-        <v>359</v>
+        <v>460</v>
       </c>
       <c r="C179" t="s">
-        <v>361</v>
-      </c>
-      <c r="E179" t="s">
-        <v>535</v>
+        <v>656</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>659</v>
       </c>
       <c r="F179" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>356</v>
+        <v>652</v>
+      </c>
+      <c r="G179" s="4"/>
+    </row>
+    <row r="180" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B180" t="s">
-        <v>58</v>
+        <v>460</v>
       </c>
       <c r="C180" t="s">
-        <v>455</v>
-      </c>
-      <c r="E180" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>356</v>
+        <v>653</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="F180" t="s">
+        <v>653</v>
+      </c>
+      <c r="G180" s="4"/>
+    </row>
+    <row r="181" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B181" t="s">
-        <v>58</v>
+        <v>460</v>
       </c>
       <c r="C181" t="s">
-        <v>456</v>
-      </c>
-      <c r="E181" t="s">
-        <v>536</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="F181" t="s">
+        <v>654</v>
+      </c>
+      <c r="G181" s="4"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B182" t="s">
-        <v>321</v>
+        <v>359</v>
       </c>
       <c r="C182" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="E182" t="s">
-        <v>534</v>
+        <v>319</v>
       </c>
       <c r="F182" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B183" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C183" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="E183" t="s">
-        <v>323</v>
+        <v>535</v>
       </c>
       <c r="F183" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5604,16 +5648,13 @@
         <v>356</v>
       </c>
       <c r="B184" t="s">
-        <v>358</v>
+        <v>58</v>
       </c>
       <c r="C184" t="s">
-        <v>324</v>
+        <v>455</v>
       </c>
       <c r="E184" t="s">
-        <v>325</v>
-      </c>
-      <c r="F184" t="s">
-        <v>542</v>
+        <v>320</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -5621,16 +5662,13 @@
         <v>356</v>
       </c>
       <c r="B185" t="s">
-        <v>358</v>
+        <v>58</v>
       </c>
       <c r="C185" t="s">
-        <v>326</v>
+        <v>456</v>
       </c>
       <c r="E185" t="s">
-        <v>327</v>
-      </c>
-      <c r="F185" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -5638,16 +5676,16 @@
         <v>356</v>
       </c>
       <c r="B186" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="C186" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E186" t="s">
-        <v>329</v>
+        <v>534</v>
       </c>
       <c r="F186" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -5658,13 +5696,13 @@
         <v>358</v>
       </c>
       <c r="C187" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E187" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F187" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5675,13 +5713,13 @@
         <v>358</v>
       </c>
       <c r="C188" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E188" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="F188" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5692,13 +5730,13 @@
         <v>358</v>
       </c>
       <c r="C189" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="E189" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="F189" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -5709,10 +5747,13 @@
         <v>358</v>
       </c>
       <c r="C190" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E190" t="s">
-        <v>337</v>
+        <v>329</v>
+      </c>
+      <c r="F190" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -5723,78 +5764,75 @@
         <v>358</v>
       </c>
       <c r="C191" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E191" t="s">
-        <v>339</v>
+        <v>331</v>
+      </c>
+      <c r="F191" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B192" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C192" t="s">
-        <v>2</v>
+        <v>332</v>
       </c>
       <c r="E192" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="F192" t="s">
-        <v>28</v>
+        <v>545</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B193" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C193" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
       <c r="E193" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F193" t="s">
-        <v>27</v>
+        <v>546</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B194" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C194" t="s">
-        <v>215</v>
+        <v>336</v>
       </c>
       <c r="E194" t="s">
-        <v>342</v>
-      </c>
-      <c r="F194" t="s">
-        <v>8</v>
+        <v>337</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B195" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C195" t="s">
-        <v>22</v>
+        <v>338</v>
       </c>
       <c r="E195" t="s">
-        <v>343</v>
-      </c>
-      <c r="F195" t="s">
-        <v>11</v>
+        <v>339</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -5805,13 +5843,13 @@
         <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>363</v>
+        <v>2</v>
       </c>
       <c r="E196" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F196" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -5822,81 +5860,81 @@
         <v>1</v>
       </c>
       <c r="C197" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E197" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F197" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B198" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>112</v>
+        <v>215</v>
       </c>
       <c r="E198" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="F198" t="s">
-        <v>388</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B199" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C199" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E199" t="s">
-        <v>389</v>
+        <v>343</v>
       </c>
       <c r="F199" t="s">
-        <v>390</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B200" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C200" t="s">
-        <v>56</v>
+        <v>363</v>
       </c>
       <c r="E200" t="s">
-        <v>391</v>
+        <v>344</v>
       </c>
       <c r="F200" t="s">
-        <v>392</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B201" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C201" t="s">
-        <v>426</v>
+        <v>364</v>
       </c>
       <c r="E201" t="s">
-        <v>393</v>
+        <v>345</v>
       </c>
       <c r="F201" t="s">
-        <v>394</v>
+        <v>18</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -5907,13 +5945,13 @@
         <v>303</v>
       </c>
       <c r="C202" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="E202" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="F202" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -5924,13 +5962,13 @@
         <v>303</v>
       </c>
       <c r="C203" t="s">
-        <v>428</v>
+        <v>54</v>
       </c>
       <c r="E203" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="F203" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -5941,13 +5979,13 @@
         <v>303</v>
       </c>
       <c r="C204" t="s">
-        <v>427</v>
+        <v>56</v>
       </c>
       <c r="E204" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="F204" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -5958,13 +5996,13 @@
         <v>303</v>
       </c>
       <c r="C205" t="s">
-        <v>174</v>
+        <v>426</v>
       </c>
       <c r="E205" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="F205" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5975,13 +6013,13 @@
         <v>303</v>
       </c>
       <c r="C206" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E206" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="F206" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -5992,13 +6030,13 @@
         <v>303</v>
       </c>
       <c r="C207" t="s">
-        <v>90</v>
+        <v>428</v>
       </c>
       <c r="E207" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="F207" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -6006,16 +6044,16 @@
         <v>357</v>
       </c>
       <c r="B208" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C208" t="s">
-        <v>112</v>
+        <v>427</v>
       </c>
       <c r="E208" t="s">
-        <v>365</v>
+        <v>399</v>
       </c>
       <c r="F208" t="s">
-        <v>366</v>
+        <v>400</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -6023,16 +6061,16 @@
         <v>357</v>
       </c>
       <c r="B209" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C209" t="s">
-        <v>54</v>
+        <v>174</v>
       </c>
       <c r="E209" t="s">
-        <v>367</v>
+        <v>401</v>
       </c>
       <c r="F209" t="s">
-        <v>368</v>
+        <v>402</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -6040,16 +6078,16 @@
         <v>357</v>
       </c>
       <c r="B210" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C210" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="E210" t="s">
-        <v>369</v>
+        <v>403</v>
       </c>
       <c r="F210" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -6057,16 +6095,16 @@
         <v>357</v>
       </c>
       <c r="B211" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C211" t="s">
-        <v>427</v>
+        <v>90</v>
       </c>
       <c r="E211" t="s">
-        <v>371</v>
+        <v>405</v>
       </c>
       <c r="F211" t="s">
-        <v>372</v>
+        <v>406</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -6077,13 +6115,13 @@
         <v>304</v>
       </c>
       <c r="C212" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="E212" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="F212" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -6094,13 +6132,13 @@
         <v>304</v>
       </c>
       <c r="C213" t="s">
-        <v>141</v>
+        <v>54</v>
       </c>
       <c r="E213" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="F213" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -6111,13 +6149,13 @@
         <v>304</v>
       </c>
       <c r="C214" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="E214" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="F214" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -6128,13 +6166,13 @@
         <v>304</v>
       </c>
       <c r="C215" t="s">
-        <v>162</v>
+        <v>427</v>
       </c>
       <c r="E215" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="F215" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -6145,13 +6183,13 @@
         <v>304</v>
       </c>
       <c r="C216" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="E216" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="F216" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
@@ -6162,13 +6200,13 @@
         <v>304</v>
       </c>
       <c r="C217" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="E217" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="F217" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
@@ -6179,13 +6217,13 @@
         <v>304</v>
       </c>
       <c r="C218" t="s">
-        <v>177</v>
+        <v>90</v>
       </c>
       <c r="E218" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="F218" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -6193,16 +6231,16 @@
         <v>357</v>
       </c>
       <c r="B219" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C219" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="E219" t="s">
-        <v>346</v>
+        <v>379</v>
       </c>
       <c r="F219" t="s">
-        <v>439</v>
+        <v>380</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -6210,16 +6248,16 @@
         <v>357</v>
       </c>
       <c r="B220" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C220" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="E220" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="F220" t="s">
-        <v>438</v>
+        <v>382</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -6227,16 +6265,16 @@
         <v>357</v>
       </c>
       <c r="B221" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C221" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="E221" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
       <c r="F221" t="s">
-        <v>437</v>
+        <v>384</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -6244,16 +6282,16 @@
         <v>357</v>
       </c>
       <c r="B222" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C222" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="E222" t="s">
-        <v>349</v>
+        <v>385</v>
       </c>
       <c r="F222" t="s">
-        <v>436</v>
+        <v>386</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -6264,13 +6302,13 @@
         <v>305</v>
       </c>
       <c r="C223" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="E223" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F223" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -6281,13 +6319,13 @@
         <v>305</v>
       </c>
       <c r="C224" t="s">
-        <v>226</v>
+        <v>112</v>
       </c>
       <c r="E224" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F224" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -6298,13 +6336,13 @@
         <v>305</v>
       </c>
       <c r="C225" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="E225" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F225" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -6315,13 +6353,13 @@
         <v>305</v>
       </c>
       <c r="C226" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="E226" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F226" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -6332,81 +6370,81 @@
         <v>305</v>
       </c>
       <c r="C227" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="E227" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F227" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B228" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C228" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="E228" t="s">
-        <v>409</v>
+        <v>351</v>
       </c>
       <c r="F228" t="s">
-        <v>410</v>
+        <v>434</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B229" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C229" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="E229" t="s">
-        <v>411</v>
+        <v>352</v>
       </c>
       <c r="F229" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B230" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C230" t="s">
-        <v>281</v>
+        <v>230</v>
       </c>
       <c r="E230" t="s">
-        <v>413</v>
+        <v>353</v>
       </c>
       <c r="F230" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B231" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C231" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="E231" t="s">
-        <v>415</v>
+        <v>354</v>
       </c>
       <c r="F231" t="s">
-        <v>416</v>
+        <v>431</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
@@ -6417,13 +6455,13 @@
         <v>425</v>
       </c>
       <c r="C232" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E232" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="F232" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
@@ -6434,13 +6472,13 @@
         <v>425</v>
       </c>
       <c r="C233" t="s">
-        <v>430</v>
+        <v>205</v>
       </c>
       <c r="E233" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="F233" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
@@ -6448,84 +6486,84 @@
         <v>423</v>
       </c>
       <c r="B234" t="s">
-        <v>306</v>
+        <v>425</v>
       </c>
       <c r="C234" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
       <c r="E234" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="F234" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B235" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C235" t="s">
-        <v>429</v>
+        <v>283</v>
       </c>
       <c r="E235" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="F235" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B236" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="C236" t="s">
-        <v>443</v>
+        <v>290</v>
       </c>
       <c r="E236" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
       <c r="F236" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B237" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="C237" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="E237" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="F237" t="s">
-        <v>447</v>
+        <v>420</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B238" t="s">
-        <v>442</v>
+        <v>306</v>
       </c>
       <c r="C238" t="s">
-        <v>449</v>
+        <v>306</v>
       </c>
       <c r="E238" t="s">
-        <v>450</v>
+        <v>421</v>
       </c>
       <c r="F238" t="s">
-        <v>451</v>
+        <v>422</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
@@ -6533,158 +6571,146 @@
         <v>424</v>
       </c>
       <c r="B239" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C239" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="E239" t="s">
-        <v>453</v>
+        <v>407</v>
       </c>
       <c r="F239" t="s">
-        <v>454</v>
+        <v>408</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="B240" t="s">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="C240" t="s">
-        <v>463</v>
+        <v>443</v>
       </c>
       <c r="E240" t="s">
-        <v>465</v>
+        <v>444</v>
+      </c>
+      <c r="F240" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>464</v>
+      <c r="A241" t="s">
+        <v>424</v>
       </c>
       <c r="B241" t="s">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="C241" t="s">
-        <v>468</v>
+        <v>448</v>
       </c>
       <c r="E241" t="s">
-        <v>562</v>
+        <v>446</v>
+      </c>
+      <c r="F241" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>484</v>
+      <c r="A242" t="s">
+        <v>424</v>
       </c>
       <c r="B242" t="s">
-        <v>481</v>
+        <v>442</v>
       </c>
       <c r="C242" t="s">
-        <v>482</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>495</v>
+        <v>449</v>
+      </c>
+      <c r="E242" t="s">
+        <v>450</v>
       </c>
       <c r="F242" t="s">
-        <v>485</v>
+        <v>451</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>484</v>
+        <v>424</v>
       </c>
       <c r="B243" t="s">
-        <v>481</v>
+        <v>442</v>
       </c>
       <c r="C243" t="s">
-        <v>483</v>
+        <v>452</v>
       </c>
       <c r="E243" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="F243" t="s">
-        <v>486</v>
+        <v>454</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>466</v>
+      <c r="A244" t="s">
+        <v>464</v>
       </c>
       <c r="B244" t="s">
         <v>462</v>
       </c>
       <c r="C244" t="s">
-        <v>626</v>
+        <v>463</v>
       </c>
       <c r="E244" t="s">
-        <v>467</v>
-      </c>
-      <c r="F244" t="s">
-        <v>611</v>
-      </c>
-      <c r="G244" s="4" t="s">
-        <v>625</v>
+        <v>465</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B245" t="s">
         <v>462</v>
       </c>
       <c r="C245" t="s">
-        <v>627</v>
+        <v>468</v>
       </c>
       <c r="E245" t="s">
-        <v>613</v>
-      </c>
-      <c r="F245" t="s">
-        <v>612</v>
-      </c>
-      <c r="G245" s="4" t="s">
-        <v>625</v>
+        <v>562</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
       <c r="B246" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="C246" t="s">
-        <v>628</v>
-      </c>
-      <c r="E246" t="s">
-        <v>614</v>
+        <v>482</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>495</v>
       </c>
       <c r="F246" t="s">
-        <v>615</v>
-      </c>
-      <c r="G246" s="4" t="s">
-        <v>625</v>
+        <v>485</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
-        <v>466</v>
+      <c r="A247" t="s">
+        <v>484</v>
       </c>
       <c r="B247" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="C247" t="s">
-        <v>629</v>
+        <v>483</v>
       </c>
       <c r="E247" t="s">
-        <v>616</v>
+        <v>496</v>
       </c>
       <c r="F247" t="s">
-        <v>617</v>
-      </c>
-      <c r="G247" s="4" t="s">
-        <v>625</v>
+        <v>486</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -6695,13 +6721,13 @@
         <v>462</v>
       </c>
       <c r="C248" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E248" t="s">
-        <v>563</v>
+        <v>467</v>
       </c>
       <c r="F248" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="G248" s="4" t="s">
         <v>625</v>
@@ -6715,13 +6741,13 @@
         <v>462</v>
       </c>
       <c r="C249" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E249" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="F249" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="G249" s="4" t="s">
         <v>625</v>
@@ -6735,13 +6761,13 @@
         <v>462</v>
       </c>
       <c r="C250" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="E250" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="F250" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="G250" s="4" t="s">
         <v>625</v>
@@ -6755,13 +6781,13 @@
         <v>462</v>
       </c>
       <c r="C251" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="E251" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="F251" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="G251" s="4" t="s">
         <v>625</v>
@@ -6772,16 +6798,16 @@
         <v>466</v>
       </c>
       <c r="B252" t="s">
-        <v>646</v>
+        <v>462</v>
       </c>
       <c r="C252" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E252" t="s">
-        <v>635</v>
+        <v>563</v>
       </c>
       <c r="F252" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="G252" s="4" t="s">
         <v>625</v>
@@ -6792,141 +6818,149 @@
         <v>466</v>
       </c>
       <c r="B253" t="s">
+        <v>462</v>
+      </c>
+      <c r="C253" t="s">
+        <v>631</v>
+      </c>
+      <c r="E253" t="s">
+        <v>619</v>
+      </c>
+      <c r="F253" t="s">
+        <v>620</v>
+      </c>
+      <c r="G253" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B254" t="s">
+        <v>462</v>
+      </c>
+      <c r="C254" t="s">
+        <v>632</v>
+      </c>
+      <c r="E254" t="s">
+        <v>621</v>
+      </c>
+      <c r="F254" t="s">
+        <v>622</v>
+      </c>
+      <c r="G254" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B255" t="s">
+        <v>462</v>
+      </c>
+      <c r="C255" t="s">
+        <v>633</v>
+      </c>
+      <c r="E255" t="s">
+        <v>623</v>
+      </c>
+      <c r="F255" t="s">
+        <v>624</v>
+      </c>
+      <c r="G255" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B256" t="s">
         <v>646</v>
       </c>
-      <c r="C253" t="s">
-        <v>647</v>
-      </c>
-      <c r="E253" t="s">
-        <v>650</v>
-      </c>
-      <c r="F253" t="s">
-        <v>649</v>
-      </c>
-      <c r="G253" s="4" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B254" t="s">
-        <v>480</v>
-      </c>
-      <c r="C254" t="s">
-        <v>488</v>
-      </c>
-      <c r="E254" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F254" t="s">
-        <v>490</v>
-      </c>
-      <c r="G254" s="4"/>
-    </row>
-    <row r="255" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B255" t="s">
-        <v>480</v>
-      </c>
-      <c r="C255" t="s">
-        <v>489</v>
-      </c>
-      <c r="E255" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F255" t="s">
-        <v>487</v>
-      </c>
-      <c r="G255" s="4"/>
-    </row>
-    <row r="256" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B256" t="s">
-        <v>480</v>
-      </c>
       <c r="C256" t="s">
-        <v>491</v>
-      </c>
-      <c r="E256" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="G256" s="4"/>
+        <v>634</v>
+      </c>
+      <c r="E256" t="s">
+        <v>635</v>
+      </c>
+      <c r="F256" t="s">
+        <v>624</v>
+      </c>
+      <c r="G256" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B257" t="s">
-        <v>481</v>
+        <v>646</v>
       </c>
       <c r="C257" t="s">
-        <v>482</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>493</v>
+        <v>647</v>
+      </c>
+      <c r="E257" t="s">
+        <v>650</v>
       </c>
       <c r="F257" t="s">
-        <v>485</v>
-      </c>
-      <c r="G257" s="4"/>
-    </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+        <v>649</v>
+      </c>
+      <c r="G257" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B258" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C258" t="s">
-        <v>483</v>
-      </c>
-      <c r="E258" t="s">
-        <v>494</v>
+        <v>488</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>497</v>
       </c>
       <c r="F258" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="G258" s="4"/>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B259" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="C259" t="s">
-        <v>500</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>501</v>
+        <v>489</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>498</v>
       </c>
       <c r="F259" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="G259" s="4"/>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B260" t="s">
-        <v>575</v>
+        <v>480</v>
       </c>
       <c r="C260" t="s">
-        <v>572</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="F260" t="s">
-        <v>573</v>
+        <v>491</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>492</v>
       </c>
       <c r="G260" s="4"/>
     </row>
@@ -6935,70 +6969,70 @@
         <v>479</v>
       </c>
       <c r="B261" t="s">
-        <v>568</v>
+        <v>481</v>
       </c>
       <c r="C261" t="s">
-        <v>569</v>
-      </c>
-      <c r="E261" s="3" t="s">
-        <v>570</v>
+        <v>482</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>493</v>
       </c>
       <c r="F261" t="s">
-        <v>571</v>
+        <v>485</v>
       </c>
       <c r="G261" s="4"/>
     </row>
-    <row r="262" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B262" t="s">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="C262" t="s">
-        <v>508</v>
-      </c>
-      <c r="E262" s="2" t="s">
-        <v>561</v>
+        <v>483</v>
+      </c>
+      <c r="E262" t="s">
+        <v>494</v>
       </c>
       <c r="F262" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="G262" s="4"/>
     </row>
-    <row r="263" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B263" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C263" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F263" s="2" t="s">
-        <v>512</v>
+        <v>501</v>
+      </c>
+      <c r="F263" t="s">
+        <v>502</v>
       </c>
       <c r="G263" s="4"/>
     </row>
-    <row r="264" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B264" t="s">
-        <v>505</v>
+        <v>575</v>
       </c>
       <c r="C264" t="s">
-        <v>511</v>
-      </c>
-      <c r="E264" s="3" t="s">
-        <v>566</v>
+        <v>572</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>574</v>
       </c>
       <c r="F264" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="G264" s="4"/>
     </row>
@@ -7007,56 +7041,56 @@
         <v>479</v>
       </c>
       <c r="B265" t="s">
-        <v>506</v>
+        <v>568</v>
       </c>
       <c r="C265" t="s">
-        <v>513</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>560</v>
+        <v>569</v>
+      </c>
+      <c r="E265" s="3" t="s">
+        <v>570</v>
       </c>
       <c r="F265" t="s">
-        <v>514</v>
+        <v>571</v>
       </c>
       <c r="G265" s="4"/>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B266" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C266" t="s">
-        <v>515</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>516</v>
+        <v>508</v>
+      </c>
+      <c r="E266" s="2" t="s">
+        <v>561</v>
       </c>
       <c r="F266" t="s">
-        <v>526</v>
+        <v>507</v>
       </c>
       <c r="G266" s="4"/>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B267" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C267" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="F267" t="s">
-        <v>527</v>
+        <v>510</v>
+      </c>
+      <c r="F267" s="2" t="s">
+        <v>512</v>
       </c>
       <c r="G267" s="4"/>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>479</v>
       </c>
@@ -7064,13 +7098,13 @@
         <v>505</v>
       </c>
       <c r="C268" t="s">
-        <v>517</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>518</v>
+        <v>511</v>
+      </c>
+      <c r="E268" s="3" t="s">
+        <v>566</v>
       </c>
       <c r="F268" t="s">
-        <v>528</v>
+        <v>567</v>
       </c>
       <c r="G268" s="4"/>
     </row>
@@ -7079,16 +7113,16 @@
         <v>479</v>
       </c>
       <c r="B269" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C269" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>596</v>
+        <v>560</v>
       </c>
       <c r="F269" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="G269" s="4"/>
     </row>
@@ -7097,18 +7131,90 @@
         <v>479</v>
       </c>
       <c r="B270" t="s">
+        <v>505</v>
+      </c>
+      <c r="C270" t="s">
+        <v>515</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="F270" t="s">
+        <v>526</v>
+      </c>
+      <c r="G270" s="4"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B271" t="s">
+        <v>505</v>
+      </c>
+      <c r="C271" t="s">
+        <v>525</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F271" t="s">
+        <v>527</v>
+      </c>
+      <c r="G271" s="4"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B272" t="s">
+        <v>505</v>
+      </c>
+      <c r="C272" t="s">
+        <v>517</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F272" t="s">
+        <v>528</v>
+      </c>
+      <c r="G272" s="4"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B273" t="s">
+        <v>505</v>
+      </c>
+      <c r="C273" t="s">
+        <v>529</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="F273" t="s">
+        <v>530</v>
+      </c>
+      <c r="G273" s="4"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B274" t="s">
         <v>506</v>
       </c>
-      <c r="C270" t="s">
+      <c r="C274" t="s">
         <v>531</v>
       </c>
-      <c r="E270" s="1" t="s">
+      <c r="E274" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F270" t="s">
+      <c r="F274" t="s">
         <v>532</v>
       </c>
-      <c r="G270" s="4"/>
+      <c r="G274" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moved a snippet, close https://github.com/2sic/2sxc/issues/1118
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -2134,7 +2134,20 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G274" totalsRowShown="0">
-  <autoFilter ref="A1:G274"/>
+  <autoFilter ref="A1:G274">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="@\InputType"/>
+        <filter val="@App"/>
+        <filter val="@C#"/>
+        <filter val="@Content"/>
+        <filter val="@DnnRazor"/>
+        <filter val="@Html"/>
+        <filter val="@List"/>
+        <filter val="@User"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2413,8 +2426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5483,10 +5496,10 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>459</v>
+        <v>479</v>
       </c>
       <c r="B175" t="s">
-        <v>644</v>
+        <v>499</v>
       </c>
       <c r="C175" t="s">
         <v>637</v>
@@ -5609,7 +5622,7 @@
       </c>
       <c r="G181" s="4"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>355</v>
       </c>
@@ -5626,7 +5639,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>355</v>
       </c>
@@ -5643,7 +5656,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>356</v>
       </c>
@@ -5657,7 +5670,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>356</v>
       </c>
@@ -5671,7 +5684,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>356</v>
       </c>
@@ -5688,7 +5701,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>356</v>
       </c>
@@ -5705,7 +5718,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>356</v>
       </c>
@@ -5722,7 +5735,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>356</v>
       </c>
@@ -5739,7 +5752,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>356</v>
       </c>
@@ -5756,7 +5769,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>356</v>
       </c>
@@ -5773,7 +5786,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>356</v>
       </c>
@@ -5790,7 +5803,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>356</v>
       </c>
@@ -5807,7 +5820,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>356</v>
       </c>
@@ -5821,7 +5834,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>356</v>
       </c>
@@ -5835,7 +5848,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>478</v>
       </c>
@@ -5852,7 +5865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>478</v>
       </c>
@@ -5869,7 +5882,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>478</v>
       </c>
@@ -5886,7 +5899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>478</v>
       </c>
@@ -5903,7 +5916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>478</v>
       </c>
@@ -5920,7 +5933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>478</v>
       </c>
@@ -5937,7 +5950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5954,7 +5967,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5971,7 +5984,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5988,7 +6001,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -6005,7 +6018,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -6022,7 +6035,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -6039,7 +6052,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -6056,7 +6069,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -6073,7 +6086,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -6090,7 +6103,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -6107,7 +6120,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -6124,7 +6137,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -6141,7 +6154,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -6158,7 +6171,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -6175,7 +6188,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -6192,7 +6205,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>357</v>
       </c>
@@ -6209,7 +6222,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>357</v>
       </c>
@@ -6226,7 +6239,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>357</v>
       </c>
@@ -6243,7 +6256,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>357</v>
       </c>
@@ -6260,7 +6273,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>357</v>
       </c>
@@ -6277,7 +6290,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>357</v>
       </c>
@@ -6294,7 +6307,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>357</v>
       </c>
@@ -6311,7 +6324,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>357</v>
       </c>
@@ -6328,7 +6341,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>357</v>
       </c>
@@ -6345,7 +6358,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>357</v>
       </c>
@@ -6362,7 +6375,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>357</v>
       </c>
@@ -6379,7 +6392,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>357</v>
       </c>
@@ -6396,7 +6409,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>357</v>
       </c>
@@ -6413,7 +6426,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>357</v>
       </c>
@@ -6430,7 +6443,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>357</v>
       </c>
@@ -6447,7 +6460,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>423</v>
       </c>
@@ -6464,7 +6477,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>423</v>
       </c>
@@ -6481,7 +6494,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>423</v>
       </c>
@@ -6498,7 +6511,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>423</v>
       </c>
@@ -6515,7 +6528,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>423</v>
       </c>
@@ -6532,7 +6545,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>423</v>
       </c>
@@ -6549,7 +6562,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>423</v>
       </c>
@@ -6566,7 +6579,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>424</v>
       </c>
@@ -6583,7 +6596,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>424</v>
       </c>
@@ -6600,7 +6613,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>424</v>
       </c>
@@ -6617,7 +6630,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>424</v>
       </c>
@@ -6634,7 +6647,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>424</v>
       </c>
@@ -6651,7 +6664,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>464</v>
       </c>
@@ -6665,7 +6678,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>464</v>
       </c>
@@ -6679,7 +6692,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>484</v>
       </c>
@@ -6696,7 +6709,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>484</v>
       </c>

</xml_diff>

<commit_message>
created Koi snippets :)
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="723">
   <si>
     <t>set</t>
   </si>
@@ -2070,6 +2070,196 @@
   </si>
   <si>
     <t>@RenderPage("_${1:list-item}.cshtml")</t>
+  </si>
+  <si>
+    <t>@using Connect.Koi;</t>
+  </si>
+  <si>
+    <t>Get CSS Framework Code</t>
+  </si>
+  <si>
+    <t>Show something if unknown</t>
+  </si>
+  <si>
+    <t>Pick a supported framework code, or use fallback</t>
+  </si>
+  <si>
+    <t>Include a CSS file of one of a supported framework</t>
+  </si>
+  <si>
+    <t>@Koi.Css</t>
+  </si>
+  <si>
+    <t>Shows the current css-framework code - requires the @using somewhere in the file.</t>
+  </si>
+  <si>
+    <t>Returns the css-code of the list you support, or returns another value if not</t>
+  </si>
+  <si>
+    <t>Outputs this text if the framework isn't known</t>
+  </si>
+  <si>
+    <t>Check if the skin doesn't publish the framework</t>
+  </si>
+  <si>
+    <t>@Koi.IsUnknown</t>
+  </si>
+  <si>
+    <t>Returns true if unknown, false if known.</t>
+  </si>
+  <si>
+    <t>Outputs this text if the framework isn't known or the other one if known</t>
+  </si>
+  <si>
+    <t>If unknown or known</t>
+  </si>
+  <si>
+    <t>@Koi.IfUnknown("&lt;link rel='stylesheet' href='https://maxcdn.bootstrapcdn.com/bootstrap/3.3.7/css/bootstrap.min.css'&gt;")</t>
+  </si>
+  <si>
+    <t>@Koi.IfUnknown("&lt;link rel='stylesheet' href='https://maxcdn.bootstrapcdn.com/bootstrap/4.0.0/css/bootstrap.min.css' integrity='sha384-Gn5384xqQ1aoWXA+058RXPxPg6fy4IWvTNh0E263XmFcJlSAwiGgFAW/dAiS6JXm' crossorigin='anonymous'&gt;")</t>
+  </si>
+  <si>
+    <t>Include bootstrap 3 from a CDN if the theme doesn't publish it's framework.</t>
+  </si>
+  <si>
+    <t>Include bootstrap 4 from a CDN if the theme doesn't publish it's framework.</t>
+  </si>
+  <si>
+    <t>@Koi.PickCss("${1:bs3,bs4,fnd6}", "${2:other}")</t>
+  </si>
+  <si>
+    <t>@Koi.IfUnknown("${1:css framework unknown}")</t>
+  </si>
+  <si>
+    <t>@Koi.IfUnknown("${1:css framework unknown}", "${2:it is defined!}")</t>
+  </si>
+  <si>
+    <t>@Koi.Class("all='ga-albums' bs3='row' bs4='row4'")</t>
+  </si>
+  <si>
+    <t>Class attr. for bootstrap 3, 4 and unknown</t>
+  </si>
+  <si>
+    <t>Class attr. for bootstrap 3, 4</t>
+  </si>
+  <si>
+    <t>Example for a simple bootstrap3 and 4 difference</t>
+  </si>
+  <si>
+    <t>Example for a simple bootstrap3 and 4 difference + unknown</t>
+  </si>
+  <si>
+    <t>Example for shared classes, bs3/4</t>
+  </si>
+  <si>
+    <t>Show a section if supported framework</t>
+  </si>
+  <si>
+    <t>Show something short if a supported framework</t>
+  </si>
+  <si>
+    <t>@Koi.If("${1:bs3,bs4}", "${2:&lt;strong&gt;supported&lt;/strong&gt;}")</t>
+  </si>
+  <si>
+    <t>http://connect-koi.net/components</t>
+  </si>
+  <si>
+    <t>Show something short if a supported, otherwise show something else</t>
+  </si>
+  <si>
+    <t>Show a text or short html if it's a supported framework.</t>
+  </si>
+  <si>
+    <t>Show a text or short html if it's a supported framework; otherwise show something else.</t>
+  </si>
+  <si>
+    <t>Include bootstrap 4 from a CDN if the theme isn't Bootstrap 3/4</t>
+  </si>
+  <si>
+    <t>Include bootstrap 3 from a CDN if the theme theme isn't Bootstrap 3/4</t>
+  </si>
+  <si>
+    <t>@Koi.If("${1:bs3,bs4}", "", "&lt;link rel='stylesheet' href='https://maxcdn.bootstrapcdn.com/bootstrap/3.3.7/css/bootstrap.min.css'&gt;")</t>
+  </si>
+  <si>
+    <t>@Koi.If("${1:bs3,bs4}", "", "&lt;link rel='stylesheet' href='https://maxcdn.bootstrapcdn.com/bootstrap/4.0.0/css/bootstrap.min.css' integrity='sha384-Gn5384xqQ1aoWXA+058RXPxPg6fy4IWvTNh0E263XmFcJlSAwiGgFAW/dAiS6JXm' crossorigin='anonymous'&gt;")</t>
+  </si>
+  <si>
+    <t>@Koi.Class("bs3='${1:row}' bs4='${2:row}'")</t>
+  </si>
+  <si>
+    <t>@Koi.Class("bs3='${1:row}' bs4='${2:row}' unk='${3:unknown}'")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class attr. for BS 3, 4 and all </t>
+  </si>
+  <si>
+    <t>Class attr. for bs3/4 - with all others reverting to BS3</t>
+  </si>
+  <si>
+    <t>@Koi.Class("all='ga-albums' bs3,oth='row' bs4='row4'")</t>
+  </si>
+  <si>
+    <t>Example where unknown or other frameworks would get the same classes as BS3</t>
+  </si>
+  <si>
+    <t>Will include bs3.css, bs4.css or fallback.css</t>
+  </si>
+  <si>
+    <t>@if(Koi.Is("${1:bs3,bs4}")) {
+    ${2:&lt;strong&gt;supported&lt;/strong&gt;}
+}</t>
+  </si>
+  <si>
+    <t>Using</t>
+  </si>
+  <si>
+    <t>IsUnknown</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>If</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>@Koi</t>
+  </si>
+  <si>
+    <t>Show a section if not supported framework</t>
+  </si>
+  <si>
+    <t>@if(!Koi.Is("${1:bs3,bs4}")) {
+    ${2:&lt;strong&gt;supported&lt;/strong&gt;}
+}</t>
+  </si>
+  <si>
+    <t>CssFramework</t>
+  </si>
+  <si>
+    <t>GetFromCdn</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href='@App.Path/dist/@(Koi.PickCss("${1:bs3,bs4}", "${2:fallback}")).css' data-enableoptimizations="true" /&gt;</t>
+  </si>
+  <si>
+    <t>Get Bootstrap3 if unknown</t>
+  </si>
+  <si>
+    <t>Get Bootstrap4 if unknown</t>
+  </si>
+  <si>
+    <t>Get Bootstrap3 if not bs3/4</t>
+  </si>
+  <si>
+    <t>Get Bootstrap4 if not bs3/4</t>
+  </si>
+  <si>
+    <t>@Koi.If("${1:bs3,bs4}", "${2:&lt;strong&gt;supported&lt;/strong&gt;}", "${3:&lt;em&gt;not supported&lt;/em&gt;}")</t>
   </si>
 </sst>
 </file>
@@ -2133,8 +2323,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G274" totalsRowShown="0">
-  <autoFilter ref="A1:G274"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G292" totalsRowShown="0">
+  <autoFilter ref="A1:G292"/>
   <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2411,10 +2601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G274"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="E198" sqref="E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5457,9 +5647,20 @@
         <v>459</v>
       </c>
       <c r="B173" t="s">
-        <v>460</v>
-      </c>
-      <c r="G173" s="4"/>
+        <v>644</v>
+      </c>
+      <c r="C173" t="s">
+        <v>638</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="F173" t="s">
+        <v>639</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
@@ -5469,39 +5670,37 @@
         <v>644</v>
       </c>
       <c r="C174" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="F174" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="G174" s="4" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B175" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C175" t="s">
-        <v>637</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>643</v>
+        <v>576</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>578</v>
       </c>
       <c r="F175" t="s">
-        <v>640</v>
-      </c>
-      <c r="G175" s="4" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+      <c r="G175" s="4"/>
+    </row>
+    <row r="176" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>459</v>
       </c>
@@ -5509,35 +5708,35 @@
         <v>645</v>
       </c>
       <c r="C176" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="F176" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G176" s="4"/>
     </row>
-    <row r="177" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B177" t="s">
-        <v>645</v>
+        <v>460</v>
       </c>
       <c r="C177" t="s">
-        <v>577</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>580</v>
+        <v>655</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>660</v>
       </c>
       <c r="F177" t="s">
-        <v>579</v>
+        <v>651</v>
       </c>
       <c r="G177" s="4"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>459</v>
       </c>
@@ -5545,17 +5744,17 @@
         <v>460</v>
       </c>
       <c r="C178" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F178" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="G178" s="4"/>
     </row>
-    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>459</v>
       </c>
@@ -5563,13 +5762,13 @@
         <v>460</v>
       </c>
       <c r="C179" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="F179" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="G179" s="4"/>
     </row>
@@ -5581,666 +5780,713 @@
         <v>460</v>
       </c>
       <c r="C180" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F180" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="G180" s="4"/>
     </row>
-    <row r="181" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>459</v>
+        <v>712</v>
       </c>
       <c r="B181" t="s">
-        <v>460</v>
-      </c>
-      <c r="C181" t="s">
-        <v>654</v>
+        <v>707</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>661</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>658</v>
-      </c>
-      <c r="F181" t="s">
-        <v>654</v>
-      </c>
-      <c r="G181" s="4"/>
+        <v>661</v>
+      </c>
+      <c r="G181" s="4" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="A182" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B182" t="s">
+        <v>715</v>
+      </c>
+      <c r="C182" t="s">
+        <v>662</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="F182" t="s">
+        <v>667</v>
+      </c>
+      <c r="G182" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B183" t="s">
+        <v>715</v>
+      </c>
+      <c r="C183" t="s">
+        <v>664</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="F183" t="s">
+        <v>668</v>
+      </c>
+      <c r="G183" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B184" t="s">
+        <v>708</v>
+      </c>
+      <c r="C184" t="s">
+        <v>670</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="F184" t="s">
+        <v>672</v>
+      </c>
+      <c r="G184" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B185" t="s">
+        <v>708</v>
+      </c>
+      <c r="C185" t="s">
+        <v>663</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F185" t="s">
+        <v>669</v>
+      </c>
+      <c r="G185" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B186" t="s">
+        <v>708</v>
+      </c>
+      <c r="C186" t="s">
+        <v>674</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="F186" t="s">
+        <v>673</v>
+      </c>
+      <c r="G186" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B187" t="s">
+        <v>716</v>
+      </c>
+      <c r="C187" t="s">
+        <v>718</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="F187" t="s">
+        <v>677</v>
+      </c>
+      <c r="G187" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B188" t="s">
+        <v>716</v>
+      </c>
+      <c r="C188" t="s">
+        <v>719</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="F188" t="s">
+        <v>678</v>
+      </c>
+      <c r="G188" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B189" t="s">
+        <v>716</v>
+      </c>
+      <c r="C189" t="s">
+        <v>720</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="F189" t="s">
+        <v>696</v>
+      </c>
+      <c r="G189" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B190" t="s">
+        <v>716</v>
+      </c>
+      <c r="C190" t="s">
+        <v>721</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="F190" t="s">
+        <v>695</v>
+      </c>
+      <c r="G190" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B191" t="s">
+        <v>711</v>
+      </c>
+      <c r="C191" t="s">
+        <v>665</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="F191" t="s">
+        <v>705</v>
+      </c>
+      <c r="G191" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B192" t="s">
+        <v>709</v>
+      </c>
+      <c r="C192" t="s">
+        <v>684</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="F192" t="s">
+        <v>685</v>
+      </c>
+      <c r="G192" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B193" t="s">
+        <v>709</v>
+      </c>
+      <c r="C193" t="s">
+        <v>683</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="F193" t="s">
+        <v>686</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B194" t="s">
+        <v>709</v>
+      </c>
+      <c r="C194" t="s">
+        <v>701</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F194" t="s">
+        <v>687</v>
+      </c>
+      <c r="G194" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B195" t="s">
+        <v>709</v>
+      </c>
+      <c r="C195" t="s">
+        <v>702</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="F195" t="s">
+        <v>704</v>
+      </c>
+      <c r="G195" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B196" t="s">
+        <v>710</v>
+      </c>
+      <c r="C196" t="s">
+        <v>689</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="F196" t="s">
+        <v>693</v>
+      </c>
+      <c r="G196" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B197" t="s">
+        <v>710</v>
+      </c>
+      <c r="C197" t="s">
+        <v>692</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="F197" t="s">
+        <v>694</v>
+      </c>
+      <c r="G197" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B198" t="s">
+        <v>710</v>
+      </c>
+      <c r="C198" t="s">
+        <v>688</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="G198" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B199" t="s">
+        <v>710</v>
+      </c>
+      <c r="C199" t="s">
+        <v>713</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="G199" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>355</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B200" t="s">
         <v>359</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C200" t="s">
         <v>360</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E200" t="s">
         <v>319</v>
       </c>
-      <c r="F182" t="s">
+      <c r="F200" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>355</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B201" t="s">
         <v>359</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C201" t="s">
         <v>361</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E201" t="s">
         <v>535</v>
       </c>
-      <c r="F183" t="s">
+      <c r="F201" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>356</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B202" t="s">
         <v>58</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C202" t="s">
         <v>455</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E202" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>356</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B203" t="s">
         <v>58</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C203" t="s">
         <v>456</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E203" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>356</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B204" t="s">
         <v>321</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C204" t="s">
         <v>321</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E204" t="s">
         <v>534</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F204" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>356</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B205" t="s">
         <v>358</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C205" t="s">
         <v>322</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E205" t="s">
         <v>323</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F205" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>356</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B206" t="s">
         <v>358</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C206" t="s">
         <v>324</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E206" t="s">
         <v>325</v>
       </c>
-      <c r="F188" t="s">
+      <c r="F206" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>356</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B207" t="s">
         <v>358</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C207" t="s">
         <v>326</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E207" t="s">
         <v>327</v>
       </c>
-      <c r="F189" t="s">
+      <c r="F207" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>356</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B208" t="s">
         <v>358</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C208" t="s">
         <v>328</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E208" t="s">
         <v>329</v>
       </c>
-      <c r="F190" t="s">
+      <c r="F208" t="s">
         <v>539</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>356</v>
-      </c>
-      <c r="B191" t="s">
-        <v>358</v>
-      </c>
-      <c r="C191" t="s">
-        <v>330</v>
-      </c>
-      <c r="E191" t="s">
-        <v>331</v>
-      </c>
-      <c r="F191" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>356</v>
-      </c>
-      <c r="B192" t="s">
-        <v>358</v>
-      </c>
-      <c r="C192" t="s">
-        <v>332</v>
-      </c>
-      <c r="E192" t="s">
-        <v>333</v>
-      </c>
-      <c r="F192" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>356</v>
-      </c>
-      <c r="B193" t="s">
-        <v>358</v>
-      </c>
-      <c r="C193" t="s">
-        <v>334</v>
-      </c>
-      <c r="E193" t="s">
-        <v>335</v>
-      </c>
-      <c r="F193" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>356</v>
-      </c>
-      <c r="B194" t="s">
-        <v>358</v>
-      </c>
-      <c r="C194" t="s">
-        <v>336</v>
-      </c>
-      <c r="E194" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>356</v>
-      </c>
-      <c r="B195" t="s">
-        <v>358</v>
-      </c>
-      <c r="C195" t="s">
-        <v>338</v>
-      </c>
-      <c r="E195" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>478</v>
-      </c>
-      <c r="B196" t="s">
-        <v>1</v>
-      </c>
-      <c r="C196" t="s">
-        <v>2</v>
-      </c>
-      <c r="E196" t="s">
-        <v>340</v>
-      </c>
-      <c r="F196" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>478</v>
-      </c>
-      <c r="B197" t="s">
-        <v>1</v>
-      </c>
-      <c r="C197" t="s">
-        <v>362</v>
-      </c>
-      <c r="E197" t="s">
-        <v>341</v>
-      </c>
-      <c r="F197" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>478</v>
-      </c>
-      <c r="B198" t="s">
-        <v>1</v>
-      </c>
-      <c r="C198" t="s">
-        <v>215</v>
-      </c>
-      <c r="E198" t="s">
-        <v>342</v>
-      </c>
-      <c r="F198" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>478</v>
-      </c>
-      <c r="B199" t="s">
-        <v>1</v>
-      </c>
-      <c r="C199" t="s">
-        <v>22</v>
-      </c>
-      <c r="E199" t="s">
-        <v>343</v>
-      </c>
-      <c r="F199" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>478</v>
-      </c>
-      <c r="B200" t="s">
-        <v>1</v>
-      </c>
-      <c r="C200" t="s">
-        <v>363</v>
-      </c>
-      <c r="E200" t="s">
-        <v>344</v>
-      </c>
-      <c r="F200" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>478</v>
-      </c>
-      <c r="B201" t="s">
-        <v>1</v>
-      </c>
-      <c r="C201" t="s">
-        <v>364</v>
-      </c>
-      <c r="E201" t="s">
-        <v>345</v>
-      </c>
-      <c r="F201" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>357</v>
-      </c>
-      <c r="B202" t="s">
-        <v>303</v>
-      </c>
-      <c r="C202" t="s">
-        <v>112</v>
-      </c>
-      <c r="E202" t="s">
-        <v>387</v>
-      </c>
-      <c r="F202" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>357</v>
-      </c>
-      <c r="B203" t="s">
-        <v>303</v>
-      </c>
-      <c r="C203" t="s">
-        <v>54</v>
-      </c>
-      <c r="E203" t="s">
-        <v>389</v>
-      </c>
-      <c r="F203" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>357</v>
-      </c>
-      <c r="B204" t="s">
-        <v>303</v>
-      </c>
-      <c r="C204" t="s">
-        <v>56</v>
-      </c>
-      <c r="E204" t="s">
-        <v>391</v>
-      </c>
-      <c r="F204" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>357</v>
-      </c>
-      <c r="B205" t="s">
-        <v>303</v>
-      </c>
-      <c r="C205" t="s">
-        <v>426</v>
-      </c>
-      <c r="E205" t="s">
-        <v>393</v>
-      </c>
-      <c r="F205" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>357</v>
-      </c>
-      <c r="B206" t="s">
-        <v>303</v>
-      </c>
-      <c r="C206" t="s">
-        <v>58</v>
-      </c>
-      <c r="E206" t="s">
-        <v>395</v>
-      </c>
-      <c r="F206" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>357</v>
-      </c>
-      <c r="B207" t="s">
-        <v>303</v>
-      </c>
-      <c r="C207" t="s">
-        <v>428</v>
-      </c>
-      <c r="E207" t="s">
-        <v>397</v>
-      </c>
-      <c r="F207" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>357</v>
-      </c>
-      <c r="B208" t="s">
-        <v>303</v>
-      </c>
-      <c r="C208" t="s">
-        <v>427</v>
-      </c>
-      <c r="E208" t="s">
-        <v>399</v>
-      </c>
-      <c r="F208" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B209" t="s">
-        <v>303</v>
+        <v>358</v>
       </c>
       <c r="C209" t="s">
-        <v>174</v>
+        <v>330</v>
       </c>
       <c r="E209" t="s">
-        <v>401</v>
+        <v>331</v>
       </c>
       <c r="F209" t="s">
-        <v>402</v>
+        <v>540</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B210" t="s">
-        <v>303</v>
+        <v>358</v>
       </c>
       <c r="C210" t="s">
-        <v>84</v>
+        <v>332</v>
       </c>
       <c r="E210" t="s">
-        <v>403</v>
+        <v>333</v>
       </c>
       <c r="F210" t="s">
-        <v>404</v>
+        <v>545</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B211" t="s">
-        <v>303</v>
+        <v>358</v>
       </c>
       <c r="C211" t="s">
-        <v>90</v>
+        <v>334</v>
       </c>
       <c r="E211" t="s">
-        <v>405</v>
+        <v>335</v>
       </c>
       <c r="F211" t="s">
-        <v>406</v>
+        <v>546</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B212" t="s">
-        <v>304</v>
+        <v>358</v>
       </c>
       <c r="C212" t="s">
-        <v>112</v>
+        <v>336</v>
       </c>
       <c r="E212" t="s">
-        <v>365</v>
-      </c>
-      <c r="F212" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B213" t="s">
-        <v>304</v>
+        <v>358</v>
       </c>
       <c r="C213" t="s">
-        <v>54</v>
+        <v>338</v>
       </c>
       <c r="E213" t="s">
-        <v>367</v>
-      </c>
-      <c r="F213" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B214" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="C214" t="s">
-        <v>115</v>
+        <v>2</v>
       </c>
       <c r="E214" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="F214" t="s">
-        <v>370</v>
+        <v>28</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B215" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="C215" t="s">
-        <v>427</v>
+        <v>362</v>
       </c>
       <c r="E215" t="s">
-        <v>371</v>
+        <v>341</v>
       </c>
       <c r="F215" t="s">
-        <v>372</v>
+        <v>27</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B216" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="C216" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
       <c r="E216" t="s">
-        <v>373</v>
+        <v>342</v>
       </c>
       <c r="F216" t="s">
-        <v>374</v>
+        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B217" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="C217" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="E217" t="s">
-        <v>375</v>
+        <v>343</v>
       </c>
       <c r="F217" t="s">
-        <v>376</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B218" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="C218" t="s">
-        <v>90</v>
+        <v>363</v>
       </c>
       <c r="E218" t="s">
-        <v>377</v>
+        <v>344</v>
       </c>
       <c r="F218" t="s">
-        <v>378</v>
+        <v>14</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B219" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>162</v>
+        <v>364</v>
       </c>
       <c r="E219" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="F219" t="s">
-        <v>380</v>
+        <v>18</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -6248,16 +6494,16 @@
         <v>357</v>
       </c>
       <c r="B220" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C220" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="E220" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="F220" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -6265,16 +6511,16 @@
         <v>357</v>
       </c>
       <c r="B221" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C221" t="s">
-        <v>174</v>
+        <v>54</v>
       </c>
       <c r="E221" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="F221" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -6282,16 +6528,16 @@
         <v>357</v>
       </c>
       <c r="B222" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C222" t="s">
-        <v>177</v>
+        <v>56</v>
       </c>
       <c r="E222" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="F222" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -6299,16 +6545,16 @@
         <v>357</v>
       </c>
       <c r="B223" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C223" t="s">
-        <v>190</v>
+        <v>426</v>
       </c>
       <c r="E223" t="s">
-        <v>346</v>
+        <v>393</v>
       </c>
       <c r="F223" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -6316,16 +6562,16 @@
         <v>357</v>
       </c>
       <c r="B224" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C224" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="E224" t="s">
-        <v>347</v>
+        <v>395</v>
       </c>
       <c r="F224" t="s">
-        <v>438</v>
+        <v>396</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -6333,16 +6579,16 @@
         <v>357</v>
       </c>
       <c r="B225" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C225" t="s">
-        <v>205</v>
+        <v>428</v>
       </c>
       <c r="E225" t="s">
-        <v>348</v>
+        <v>397</v>
       </c>
       <c r="F225" t="s">
-        <v>437</v>
+        <v>398</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -6350,16 +6596,16 @@
         <v>357</v>
       </c>
       <c r="B226" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C226" t="s">
-        <v>213</v>
+        <v>427</v>
       </c>
       <c r="E226" t="s">
-        <v>349</v>
+        <v>399</v>
       </c>
       <c r="F226" t="s">
-        <v>436</v>
+        <v>400</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -6367,16 +6613,16 @@
         <v>357</v>
       </c>
       <c r="B227" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C227" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="E227" t="s">
-        <v>350</v>
+        <v>401</v>
       </c>
       <c r="F227" t="s">
-        <v>435</v>
+        <v>402</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -6384,16 +6630,16 @@
         <v>357</v>
       </c>
       <c r="B228" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C228" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E228" t="s">
-        <v>351</v>
+        <v>403</v>
       </c>
       <c r="F228" t="s">
-        <v>434</v>
+        <v>404</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -6401,16 +6647,16 @@
         <v>357</v>
       </c>
       <c r="B229" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C229" t="s">
-        <v>234</v>
+        <v>90</v>
       </c>
       <c r="E229" t="s">
-        <v>352</v>
+        <v>405</v>
       </c>
       <c r="F229" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -6418,16 +6664,16 @@
         <v>357</v>
       </c>
       <c r="B230" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C230" t="s">
-        <v>230</v>
+        <v>112</v>
       </c>
       <c r="E230" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="F230" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -6435,786 +6681,1092 @@
         <v>357</v>
       </c>
       <c r="B231" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C231" t="s">
-        <v>262</v>
+        <v>54</v>
       </c>
       <c r="E231" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="F231" t="s">
-        <v>431</v>
+        <v>368</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B232" t="s">
-        <v>425</v>
+        <v>304</v>
       </c>
       <c r="C232" t="s">
-        <v>278</v>
+        <v>115</v>
       </c>
       <c r="E232" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="F232" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B233" t="s">
-        <v>425</v>
+        <v>304</v>
       </c>
       <c r="C233" t="s">
-        <v>205</v>
+        <v>427</v>
       </c>
       <c r="E233" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="F233" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B234" t="s">
-        <v>425</v>
+        <v>304</v>
       </c>
       <c r="C234" t="s">
-        <v>281</v>
+        <v>131</v>
       </c>
       <c r="E234" t="s">
-        <v>413</v>
+        <v>373</v>
       </c>
       <c r="F234" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B235" t="s">
-        <v>425</v>
+        <v>304</v>
       </c>
       <c r="C235" t="s">
-        <v>283</v>
+        <v>141</v>
       </c>
       <c r="E235" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="F235" t="s">
-        <v>416</v>
+        <v>376</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B236" t="s">
-        <v>425</v>
+        <v>304</v>
       </c>
       <c r="C236" t="s">
-        <v>290</v>
+        <v>90</v>
       </c>
       <c r="E236" t="s">
-        <v>417</v>
+        <v>377</v>
       </c>
       <c r="F236" t="s">
-        <v>418</v>
+        <v>378</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B237" t="s">
-        <v>425</v>
+        <v>304</v>
       </c>
       <c r="C237" t="s">
-        <v>430</v>
+        <v>162</v>
       </c>
       <c r="E237" t="s">
-        <v>419</v>
+        <v>379</v>
       </c>
       <c r="F237" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B238" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C238" t="s">
-        <v>306</v>
+        <v>166</v>
       </c>
       <c r="E238" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="F238" t="s">
-        <v>422</v>
+        <v>382</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>424</v>
+        <v>357</v>
       </c>
       <c r="B239" t="s">
-        <v>429</v>
+        <v>304</v>
       </c>
       <c r="C239" t="s">
-        <v>429</v>
+        <v>174</v>
       </c>
       <c r="E239" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="F239" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>357</v>
+      </c>
+      <c r="B240" t="s">
+        <v>304</v>
+      </c>
+      <c r="C240" t="s">
+        <v>177</v>
+      </c>
+      <c r="E240" t="s">
+        <v>385</v>
+      </c>
+      <c r="F240" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>357</v>
+      </c>
+      <c r="B241" t="s">
+        <v>305</v>
+      </c>
+      <c r="C241" t="s">
+        <v>190</v>
+      </c>
+      <c r="E241" t="s">
+        <v>346</v>
+      </c>
+      <c r="F241" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>357</v>
+      </c>
+      <c r="B242" t="s">
+        <v>305</v>
+      </c>
+      <c r="C242" t="s">
+        <v>112</v>
+      </c>
+      <c r="E242" t="s">
+        <v>347</v>
+      </c>
+      <c r="F242" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>357</v>
+      </c>
+      <c r="B243" t="s">
+        <v>305</v>
+      </c>
+      <c r="C243" t="s">
+        <v>205</v>
+      </c>
+      <c r="E243" t="s">
+        <v>348</v>
+      </c>
+      <c r="F243" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>357</v>
+      </c>
+      <c r="B244" t="s">
+        <v>305</v>
+      </c>
+      <c r="C244" t="s">
+        <v>213</v>
+      </c>
+      <c r="E244" t="s">
+        <v>349</v>
+      </c>
+      <c r="F244" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>357</v>
+      </c>
+      <c r="B245" t="s">
+        <v>305</v>
+      </c>
+      <c r="C245" t="s">
+        <v>217</v>
+      </c>
+      <c r="E245" t="s">
+        <v>350</v>
+      </c>
+      <c r="F245" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>357</v>
+      </c>
+      <c r="B246" t="s">
+        <v>305</v>
+      </c>
+      <c r="C246" t="s">
+        <v>226</v>
+      </c>
+      <c r="E246" t="s">
+        <v>351</v>
+      </c>
+      <c r="F246" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>357</v>
+      </c>
+      <c r="B247" t="s">
+        <v>305</v>
+      </c>
+      <c r="C247" t="s">
+        <v>234</v>
+      </c>
+      <c r="E247" t="s">
+        <v>352</v>
+      </c>
+      <c r="F247" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>357</v>
+      </c>
+      <c r="B248" t="s">
+        <v>305</v>
+      </c>
+      <c r="C248" t="s">
+        <v>230</v>
+      </c>
+      <c r="E248" t="s">
+        <v>353</v>
+      </c>
+      <c r="F248" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>357</v>
+      </c>
+      <c r="B249" t="s">
+        <v>305</v>
+      </c>
+      <c r="C249" t="s">
+        <v>262</v>
+      </c>
+      <c r="E249" t="s">
+        <v>354</v>
+      </c>
+      <c r="F249" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>423</v>
+      </c>
+      <c r="B250" t="s">
+        <v>425</v>
+      </c>
+      <c r="C250" t="s">
+        <v>278</v>
+      </c>
+      <c r="E250" t="s">
+        <v>409</v>
+      </c>
+      <c r="F250" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>423</v>
+      </c>
+      <c r="B251" t="s">
+        <v>425</v>
+      </c>
+      <c r="C251" t="s">
+        <v>205</v>
+      </c>
+      <c r="E251" t="s">
+        <v>411</v>
+      </c>
+      <c r="F251" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>423</v>
+      </c>
+      <c r="B252" t="s">
+        <v>425</v>
+      </c>
+      <c r="C252" t="s">
+        <v>281</v>
+      </c>
+      <c r="E252" t="s">
+        <v>413</v>
+      </c>
+      <c r="F252" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>423</v>
+      </c>
+      <c r="B253" t="s">
+        <v>425</v>
+      </c>
+      <c r="C253" t="s">
+        <v>283</v>
+      </c>
+      <c r="E253" t="s">
+        <v>415</v>
+      </c>
+      <c r="F253" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>423</v>
+      </c>
+      <c r="B254" t="s">
+        <v>425</v>
+      </c>
+      <c r="C254" t="s">
+        <v>290</v>
+      </c>
+      <c r="E254" t="s">
+        <v>417</v>
+      </c>
+      <c r="F254" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>423</v>
+      </c>
+      <c r="B255" t="s">
+        <v>425</v>
+      </c>
+      <c r="C255" t="s">
+        <v>430</v>
+      </c>
+      <c r="E255" t="s">
+        <v>419</v>
+      </c>
+      <c r="F255" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>423</v>
+      </c>
+      <c r="B256" t="s">
+        <v>306</v>
+      </c>
+      <c r="C256" t="s">
+        <v>306</v>
+      </c>
+      <c r="E256" t="s">
+        <v>421</v>
+      </c>
+      <c r="F256" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
         <v>424</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B257" t="s">
+        <v>429</v>
+      </c>
+      <c r="C257" t="s">
+        <v>429</v>
+      </c>
+      <c r="E257" t="s">
+        <v>407</v>
+      </c>
+      <c r="F257" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>424</v>
+      </c>
+      <c r="B258" t="s">
         <v>442</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C258" t="s">
         <v>443</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E258" t="s">
         <v>444</v>
       </c>
-      <c r="F240" t="s">
+      <c r="F258" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
         <v>424</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B259" t="s">
         <v>442</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C259" t="s">
         <v>448</v>
       </c>
-      <c r="E241" t="s">
+      <c r="E259" t="s">
         <v>446</v>
       </c>
-      <c r="F241" t="s">
+      <c r="F259" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
         <v>424</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B260" t="s">
         <v>442</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C260" t="s">
         <v>449</v>
       </c>
-      <c r="E242" t="s">
+      <c r="E260" t="s">
         <v>450</v>
       </c>
-      <c r="F242" t="s">
+      <c r="F260" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
         <v>424</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B261" t="s">
         <v>442</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C261" t="s">
         <v>452</v>
       </c>
-      <c r="E243" t="s">
+      <c r="E261" t="s">
         <v>453</v>
       </c>
-      <c r="F243" t="s">
+      <c r="F261" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>464</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B262" t="s">
         <v>462</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C262" t="s">
         <v>463</v>
       </c>
-      <c r="E244" t="s">
+      <c r="E262" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="B245" t="s">
-        <v>462</v>
-      </c>
-      <c r="C245" t="s">
-        <v>468</v>
-      </c>
-      <c r="E245" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B246" t="s">
-        <v>481</v>
-      </c>
-      <c r="C246" t="s">
-        <v>482</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F246" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>484</v>
-      </c>
-      <c r="B247" t="s">
-        <v>481</v>
-      </c>
-      <c r="C247" t="s">
-        <v>483</v>
-      </c>
-      <c r="E247" t="s">
-        <v>496</v>
-      </c>
-      <c r="F247" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B248" t="s">
-        <v>462</v>
-      </c>
-      <c r="C248" t="s">
-        <v>626</v>
-      </c>
-      <c r="E248" t="s">
-        <v>467</v>
-      </c>
-      <c r="F248" t="s">
-        <v>611</v>
-      </c>
-      <c r="G248" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B249" t="s">
-        <v>462</v>
-      </c>
-      <c r="C249" t="s">
-        <v>627</v>
-      </c>
-      <c r="E249" t="s">
-        <v>613</v>
-      </c>
-      <c r="F249" t="s">
-        <v>612</v>
-      </c>
-      <c r="G249" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B250" t="s">
-        <v>462</v>
-      </c>
-      <c r="C250" t="s">
-        <v>628</v>
-      </c>
-      <c r="E250" t="s">
-        <v>614</v>
-      </c>
-      <c r="F250" t="s">
-        <v>615</v>
-      </c>
-      <c r="G250" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B251" t="s">
-        <v>462</v>
-      </c>
-      <c r="C251" t="s">
-        <v>629</v>
-      </c>
-      <c r="E251" t="s">
-        <v>616</v>
-      </c>
-      <c r="F251" t="s">
-        <v>617</v>
-      </c>
-      <c r="G251" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B252" t="s">
-        <v>462</v>
-      </c>
-      <c r="C252" t="s">
-        <v>630</v>
-      </c>
-      <c r="E252" t="s">
-        <v>563</v>
-      </c>
-      <c r="F252" t="s">
-        <v>618</v>
-      </c>
-      <c r="G252" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B253" t="s">
-        <v>462</v>
-      </c>
-      <c r="C253" t="s">
-        <v>631</v>
-      </c>
-      <c r="E253" t="s">
-        <v>619</v>
-      </c>
-      <c r="F253" t="s">
-        <v>620</v>
-      </c>
-      <c r="G253" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B254" t="s">
-        <v>462</v>
-      </c>
-      <c r="C254" t="s">
-        <v>632</v>
-      </c>
-      <c r="E254" t="s">
-        <v>621</v>
-      </c>
-      <c r="F254" t="s">
-        <v>622</v>
-      </c>
-      <c r="G254" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B255" t="s">
-        <v>462</v>
-      </c>
-      <c r="C255" t="s">
-        <v>633</v>
-      </c>
-      <c r="E255" t="s">
-        <v>623</v>
-      </c>
-      <c r="F255" t="s">
-        <v>624</v>
-      </c>
-      <c r="G255" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B256" t="s">
-        <v>646</v>
-      </c>
-      <c r="C256" t="s">
-        <v>634</v>
-      </c>
-      <c r="E256" t="s">
-        <v>635</v>
-      </c>
-      <c r="F256" t="s">
-        <v>624</v>
-      </c>
-      <c r="G256" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B257" t="s">
-        <v>646</v>
-      </c>
-      <c r="C257" t="s">
-        <v>647</v>
-      </c>
-      <c r="E257" t="s">
-        <v>650</v>
-      </c>
-      <c r="F257" t="s">
-        <v>649</v>
-      </c>
-      <c r="G257" s="4" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="258" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B258" t="s">
-        <v>480</v>
-      </c>
-      <c r="C258" t="s">
-        <v>488</v>
-      </c>
-      <c r="E258" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F258" t="s">
-        <v>490</v>
-      </c>
-      <c r="G258" s="4"/>
-    </row>
-    <row r="259" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B259" t="s">
-        <v>480</v>
-      </c>
-      <c r="C259" t="s">
-        <v>489</v>
-      </c>
-      <c r="E259" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F259" t="s">
-        <v>487</v>
-      </c>
-      <c r="G259" s="4"/>
-    </row>
-    <row r="260" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B260" t="s">
-        <v>480</v>
-      </c>
-      <c r="C260" t="s">
-        <v>491</v>
-      </c>
-      <c r="E260" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="G260" s="4"/>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B261" t="s">
-        <v>481</v>
-      </c>
-      <c r="C261" t="s">
-        <v>482</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="F261" t="s">
-        <v>485</v>
-      </c>
-      <c r="G261" s="4"/>
-    </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B262" t="s">
-        <v>481</v>
-      </c>
-      <c r="C262" t="s">
-        <v>483</v>
-      </c>
-      <c r="E262" t="s">
-        <v>494</v>
-      </c>
-      <c r="F262" t="s">
-        <v>486</v>
-      </c>
-      <c r="G262" s="4"/>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="B263" t="s">
-        <v>499</v>
+        <v>462</v>
       </c>
       <c r="C263" t="s">
-        <v>500</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F263" t="s">
-        <v>502</v>
-      </c>
-      <c r="G263" s="4"/>
+        <v>468</v>
+      </c>
+      <c r="E263" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="B264" t="s">
-        <v>575</v>
+        <v>481</v>
       </c>
       <c r="C264" t="s">
-        <v>572</v>
+        <v>482</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>574</v>
+        <v>495</v>
       </c>
       <c r="F264" t="s">
-        <v>573</v>
-      </c>
-      <c r="G264" s="4"/>
+        <v>485</v>
+      </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>479</v>
+      <c r="A265" t="s">
+        <v>484</v>
       </c>
       <c r="B265" t="s">
-        <v>568</v>
+        <v>481</v>
       </c>
       <c r="C265" t="s">
-        <v>569</v>
-      </c>
-      <c r="E265" s="3" t="s">
-        <v>570</v>
+        <v>483</v>
+      </c>
+      <c r="E265" t="s">
+        <v>496</v>
       </c>
       <c r="F265" t="s">
-        <v>571</v>
-      </c>
-      <c r="G265" s="4"/>
-    </row>
-    <row r="266" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B266" t="s">
-        <v>506</v>
+        <v>462</v>
       </c>
       <c r="C266" t="s">
-        <v>508</v>
-      </c>
-      <c r="E266" s="2" t="s">
-        <v>561</v>
+        <v>626</v>
+      </c>
+      <c r="E266" t="s">
+        <v>467</v>
       </c>
       <c r="F266" t="s">
-        <v>507</v>
-      </c>
-      <c r="G266" s="4"/>
-    </row>
-    <row r="267" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>611</v>
+      </c>
+      <c r="G266" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B267" t="s">
-        <v>506</v>
+        <v>462</v>
       </c>
       <c r="C267" t="s">
-        <v>509</v>
-      </c>
-      <c r="E267" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F267" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="G267" s="4"/>
-    </row>
-    <row r="268" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+      <c r="E267" t="s">
+        <v>613</v>
+      </c>
+      <c r="F267" t="s">
+        <v>612</v>
+      </c>
+      <c r="G267" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B268" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="C268" t="s">
-        <v>511</v>
-      </c>
-      <c r="E268" s="3" t="s">
-        <v>566</v>
+        <v>628</v>
+      </c>
+      <c r="E268" t="s">
+        <v>614</v>
       </c>
       <c r="F268" t="s">
-        <v>567</v>
-      </c>
-      <c r="G268" s="4"/>
+        <v>615</v>
+      </c>
+      <c r="G268" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B269" t="s">
-        <v>506</v>
+        <v>462</v>
       </c>
       <c r="C269" t="s">
-        <v>513</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>560</v>
+        <v>629</v>
+      </c>
+      <c r="E269" t="s">
+        <v>616</v>
       </c>
       <c r="F269" t="s">
-        <v>514</v>
-      </c>
-      <c r="G269" s="4"/>
+        <v>617</v>
+      </c>
+      <c r="G269" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B270" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="C270" t="s">
-        <v>515</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>516</v>
+        <v>630</v>
+      </c>
+      <c r="E270" t="s">
+        <v>563</v>
       </c>
       <c r="F270" t="s">
-        <v>526</v>
-      </c>
-      <c r="G270" s="4"/>
+        <v>618</v>
+      </c>
+      <c r="G270" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B271" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="C271" t="s">
-        <v>525</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>518</v>
+        <v>631</v>
+      </c>
+      <c r="E271" t="s">
+        <v>619</v>
       </c>
       <c r="F271" t="s">
-        <v>527</v>
-      </c>
-      <c r="G271" s="4"/>
+        <v>620</v>
+      </c>
+      <c r="G271" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B272" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="C272" t="s">
-        <v>517</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>518</v>
+        <v>632</v>
+      </c>
+      <c r="E272" t="s">
+        <v>621</v>
       </c>
       <c r="F272" t="s">
-        <v>528</v>
-      </c>
-      <c r="G272" s="4"/>
+        <v>622</v>
+      </c>
+      <c r="G272" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B273" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="C273" t="s">
-        <v>529</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>596</v>
+        <v>633</v>
+      </c>
+      <c r="E273" t="s">
+        <v>623</v>
       </c>
       <c r="F273" t="s">
-        <v>530</v>
-      </c>
-      <c r="G273" s="4"/>
+        <v>624</v>
+      </c>
+      <c r="G273" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B274" t="s">
+        <v>646</v>
+      </c>
+      <c r="C274" t="s">
+        <v>634</v>
+      </c>
+      <c r="E274" t="s">
+        <v>635</v>
+      </c>
+      <c r="F274" t="s">
+        <v>624</v>
+      </c>
+      <c r="G274" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B275" t="s">
+        <v>646</v>
+      </c>
+      <c r="C275" t="s">
+        <v>647</v>
+      </c>
+      <c r="E275" t="s">
+        <v>650</v>
+      </c>
+      <c r="F275" t="s">
+        <v>649</v>
+      </c>
+      <c r="G275" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B276" t="s">
+        <v>480</v>
+      </c>
+      <c r="C276" t="s">
+        <v>488</v>
+      </c>
+      <c r="E276" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="F276" t="s">
+        <v>490</v>
+      </c>
+      <c r="G276" s="4"/>
+    </row>
+    <row r="277" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B277" t="s">
+        <v>480</v>
+      </c>
+      <c r="C277" t="s">
+        <v>489</v>
+      </c>
+      <c r="E277" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="F277" t="s">
+        <v>487</v>
+      </c>
+      <c r="G277" s="4"/>
+    </row>
+    <row r="278" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B278" t="s">
+        <v>480</v>
+      </c>
+      <c r="C278" t="s">
+        <v>491</v>
+      </c>
+      <c r="E278" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="G278" s="4"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B279" t="s">
+        <v>481</v>
+      </c>
+      <c r="C279" t="s">
+        <v>482</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="F279" t="s">
+        <v>485</v>
+      </c>
+      <c r="G279" s="4"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B280" t="s">
+        <v>481</v>
+      </c>
+      <c r="C280" t="s">
+        <v>483</v>
+      </c>
+      <c r="E280" t="s">
+        <v>494</v>
+      </c>
+      <c r="F280" t="s">
+        <v>486</v>
+      </c>
+      <c r="G280" s="4"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B281" t="s">
+        <v>499</v>
+      </c>
+      <c r="C281" t="s">
+        <v>500</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="F281" t="s">
+        <v>502</v>
+      </c>
+      <c r="G281" s="4"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B282" t="s">
+        <v>575</v>
+      </c>
+      <c r="C282" t="s">
+        <v>572</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="F282" t="s">
+        <v>573</v>
+      </c>
+      <c r="G282" s="4"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B283" t="s">
+        <v>568</v>
+      </c>
+      <c r="C283" t="s">
+        <v>569</v>
+      </c>
+      <c r="E283" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="F283" t="s">
+        <v>571</v>
+      </c>
+      <c r="G283" s="4"/>
+    </row>
+    <row r="284" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B284" t="s">
         <v>506</v>
       </c>
-      <c r="C274" t="s">
+      <c r="C284" t="s">
+        <v>508</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="F284" t="s">
+        <v>507</v>
+      </c>
+      <c r="G284" s="4"/>
+    </row>
+    <row r="285" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B285" t="s">
+        <v>506</v>
+      </c>
+      <c r="C285" t="s">
+        <v>509</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="F285" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="G285" s="4"/>
+    </row>
+    <row r="286" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B286" t="s">
+        <v>505</v>
+      </c>
+      <c r="C286" t="s">
+        <v>511</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F286" t="s">
+        <v>567</v>
+      </c>
+      <c r="G286" s="4"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B287" t="s">
+        <v>506</v>
+      </c>
+      <c r="C287" t="s">
+        <v>513</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F287" t="s">
+        <v>514</v>
+      </c>
+      <c r="G287" s="4"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B288" t="s">
+        <v>505</v>
+      </c>
+      <c r="C288" t="s">
+        <v>515</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="F288" t="s">
+        <v>526</v>
+      </c>
+      <c r="G288" s="4"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B289" t="s">
+        <v>505</v>
+      </c>
+      <c r="C289" t="s">
+        <v>525</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F289" t="s">
+        <v>527</v>
+      </c>
+      <c r="G289" s="4"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B290" t="s">
+        <v>505</v>
+      </c>
+      <c r="C290" t="s">
+        <v>517</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F290" t="s">
+        <v>528</v>
+      </c>
+      <c r="G290" s="4"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B291" t="s">
+        <v>505</v>
+      </c>
+      <c r="C291" t="s">
+        <v>529</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="F291" t="s">
+        <v>530</v>
+      </c>
+      <c r="G291" s="4"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B292" t="s">
+        <v>506</v>
+      </c>
+      <c r="C292" t="s">
         <v>531</v>
       </c>
-      <c r="E274" s="1" t="s">
+      <c r="E292" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F274" t="s">
+      <c r="F292" t="s">
         <v>532</v>
       </c>
-      <c r="G274" s="4"/>
+      <c r="G292" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>